<commit_message>
Repivot data in pivot sheet
</commit_message>
<xml_diff>
--- a/MeadInflowSplit/ShareOfInflow-LB-MX-SEIS.xlsx
+++ b/MeadInflowSplit/ShareOfInflow-LB-MX-SEIS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\MeadInflowSplit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA3F5B5-52DA-4DA9-BCF5-0D7E36A28C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9590CB-2F5F-474A-B63D-8BFDD641AEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" xr2:uid="{B7E24150-B936-4491-85FE-E2B15A6311EA}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{B7E24150-B936-4491-85FE-E2B15A6311EA}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="7" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="127">
   <si>
     <t>Mandatory Cutbacks according to 2007 Interim Guidelines, 2019 Drought Contingency Plan, and Minutes 319 and 323</t>
   </si>
@@ -368,9 +368,6 @@
     <t>Row Labels</t>
   </si>
   <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
     <t>Column Labels</t>
   </si>
   <si>
@@ -378,18 +375,6 @@
   </si>
   <si>
     <t>Percent of Total</t>
-  </si>
-  <si>
-    <t>Arizona Total</t>
-  </si>
-  <si>
-    <t>California Total</t>
-  </si>
-  <si>
-    <t>Mexico Total</t>
-  </si>
-  <si>
-    <t>Nevada Total</t>
   </si>
   <si>
     <t>Sum of Percent of Total</t>
@@ -538,7 +523,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -774,7 +759,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -882,70 +867,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -964,6 +901,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -971,7 +962,160 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="52">
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
     <dxf>
       <alignment wrapText="1"/>
     </dxf>
@@ -1951,24 +2095,23 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A7A995A2-5180-4438-9CFD-00C63EDBB8BA}" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="H2:Y13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A7A995A2-5180-4438-9CFD-00C63EDBB8BA}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="H2:T12" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="9">
+    <pivotField axis="axisRow" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="8">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="2"/>
         <item x="7"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField numFmtId="166" showAll="0">
-      <items count="9">
+    <pivotField numFmtId="166" showAll="0" defaultSubtotal="0">
+      <items count="8">
         <item x="7"/>
         <item x="6"/>
         <item x="5"/>
@@ -1977,32 +2120,29 @@
         <item x="2"/>
         <item x="1"/>
         <item x="0"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
       <items count="4">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
-        <item t="default"/>
+        <item x="3"/>
       </items>
     </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField dataField="1" numFmtId="9" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="8">
     <i>
       <x/>
     </i>
@@ -2027,15 +2167,12 @@
     <i>
       <x v="7"/>
     </i>
-    <i t="grand">
-      <x/>
-    </i>
   </rowItems>
   <colFields count="2">
     <field x="3"/>
     <field x="2"/>
   </colFields>
-  <colItems count="17">
+  <colItems count="12">
     <i>
       <x/>
       <x/>
@@ -2045,9 +2182,6 @@
     </i>
     <i r="1">
       <x v="2"/>
-    </i>
-    <i t="default">
-      <x/>
     </i>
     <i>
       <x v="1"/>
@@ -2059,9 +2193,6 @@
     <i r="1">
       <x v="2"/>
     </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
     <i>
       <x v="2"/>
       <x/>
@@ -2070,9 +2201,6 @@
       <x v="1"/>
     </i>
     <i r="1">
-      <x v="2"/>
-    </i>
-    <i t="default">
       <x v="2"/>
     </i>
     <i>
@@ -2085,25 +2213,94 @@
     <i r="1">
       <x v="2"/>
     </i>
-    <i t="default">
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of Percent of Total" fld="4" baseField="0" baseItem="0" numFmtId="169"/>
+    <dataField name="Sum of Percent of Total" fld="4" baseField="0" baseItem="0" numFmtId="9"/>
   </dataFields>
-  <formats count="1">
-    <format dxfId="0">
+  <formats count="12">
+    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1">
-            <x v="2"/>
+            <x v="0"/>
           </reference>
           <reference field="3" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="48">
+      <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="45">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="44">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="43">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="42">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
+    </format>
+    <format dxfId="41">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="40">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="39">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0"/>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="38">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0"/>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="37">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0"/>
+          <reference field="3" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="36">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0"/>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -2115,7 +2312,7 @@
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -2421,7 +2618,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2431,57 +2628,57 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -2491,88 +2688,88 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B27" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C29" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C30" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C31" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C32" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C33" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C34" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2584,10 +2781,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13C3540-FD7C-4DA9-A592-A207CAA87CF1}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:Y98"/>
+  <dimension ref="A2:T98"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L2" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2596,21 +2793,18 @@
     <col min="2" max="2" width="9.7265625" customWidth="1"/>
     <col min="3" max="3" width="41.6328125" customWidth="1"/>
     <col min="4" max="4" width="13.36328125" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" customWidth="1"/>
     <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.90625" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.36328125" customWidth="1"/>
-    <col min="16" max="16" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.81640625" customWidth="1"/>
-    <col min="20" max="20" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.08984375" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="18.453125" customWidth="1"/>
     <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
@@ -2678,12 +2872,12 @@
     <col min="110" max="111" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="71" t="str">
+    <row r="2" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="55" t="str">
         <f>'ShareOfInflow-SEIS'!A10</f>
         <v>Mead Elevation (feet)</v>
       </c>
-      <c r="B2" s="71" t="str">
+      <c r="B2" s="55" t="str">
         <f>'ShareOfInflow-SEIS'!B10</f>
         <v>Mead Volume (maf)</v>
       </c>
@@ -2691,19 +2885,19 @@
         <v>90</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="H2" s="73" t="s">
-        <v>100</v>
-      </c>
-      <c r="I2" s="73" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="I2" s="74" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>'ShareOfInflow-SEIS'!A12</f>
         <v>1,090–&gt;1,075</v>
@@ -2719,39 +2913,24 @@
       <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="72">
+      <c r="E3" s="56">
         <f>'ShareOfInflow-SEIS'!C12</f>
         <v>0.2822759668185536</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L3" t="s">
-        <v>96</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="L3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P3" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="R3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="T3" t="s">
-        <v>98</v>
-      </c>
-      <c r="U3" t="s">
-        <v>19</v>
-      </c>
-      <c r="X3" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>'ShareOfInflow-SEIS'!A13</f>
         <v>1,075–1,050</v>
@@ -2767,51 +2946,51 @@
       <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="72">
+      <c r="E4" s="56">
         <f>'ShareOfInflow-SEIS'!C13</f>
         <v>0.22625413801884389</v>
       </c>
-      <c r="H4" s="73" t="s">
+      <c r="H4" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="L4" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="P4" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="R4" t="s">
+      <c r="Q4" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="S4" t="s">
+      <c r="R4" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="U4" t="s">
+      <c r="S4" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="V4" t="s">
+      <c r="T4" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="W4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>'ShareOfInflow-SEIS'!A14</f>
         <v>&lt;1,050–&gt;1,045</v>
@@ -2827,66 +3006,51 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="72">
+      <c r="E5" s="56">
         <f>'ShareOfInflow-SEIS'!C14</f>
         <v>0.2107804750717828</v>
       </c>
-      <c r="H5" s="74" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" s="59">
-        <v>0.1620384498016478</v>
-      </c>
-      <c r="J5" s="59">
-        <v>0.25790424570912374</v>
-      </c>
-      <c r="K5" s="59">
-        <v>0.31877394636015327</v>
-      </c>
-      <c r="L5" s="59">
-        <v>0.73871664187092478</v>
-      </c>
-      <c r="M5" s="59">
-        <v>0.61794324076899609</v>
-      </c>
-      <c r="N5" s="59">
-        <v>0.52288467329117749</v>
-      </c>
-      <c r="O5" s="59">
-        <v>0.62068965517241392</v>
-      </c>
-      <c r="P5" s="59">
-        <v>1.7615175692325875</v>
-      </c>
-      <c r="Q5" s="59">
-        <v>0.18690875801037535</v>
-      </c>
-      <c r="R5" s="59">
-        <v>0.18443239987955437</v>
-      </c>
-      <c r="S5" s="59">
-        <v>0.18773946360153257</v>
-      </c>
-      <c r="T5" s="59">
-        <v>0.55908062149146232</v>
-      </c>
-      <c r="U5" s="59">
-        <v>3.3109551418980768E-2</v>
-      </c>
-      <c r="V5" s="59">
-        <v>3.4778681120144532E-2</v>
-      </c>
-      <c r="W5" s="59">
-        <v>4.1379310344827586E-2</v>
-      </c>
-      <c r="X5" s="59">
-        <v>0.10926754288395288</v>
-      </c>
-      <c r="Y5" s="59">
-        <v>3.1685823754789273</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="H5" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="76">
+        <v>0.30470849398294192</v>
+      </c>
+      <c r="J5" s="76">
+        <v>0.2822759668185536</v>
+      </c>
+      <c r="K5" s="76">
+        <v>0.29594578805935273</v>
+      </c>
+      <c r="L5" s="76">
+        <v>3.4116135062507304E-2</v>
+      </c>
+      <c r="M5" s="76">
+        <v>3.3181446430657784E-2</v>
+      </c>
+      <c r="N5" s="76">
+        <v>3.3181446430657784E-2</v>
+      </c>
+      <c r="O5" s="76">
+        <v>0.51407874751723337</v>
+      </c>
+      <c r="P5" s="76">
+        <v>0.51407874751723337</v>
+      </c>
+      <c r="Q5" s="76">
+        <v>0.5004089262764343</v>
+      </c>
+      <c r="R5" s="76">
+        <v>0.17046383923355535</v>
+      </c>
+      <c r="S5" s="76">
+        <v>0.17046383923355535</v>
+      </c>
+      <c r="T5" s="76">
+        <v>0.17046383923355535</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>'ShareOfInflow-SEIS'!A15</f>
         <v>1,045–&gt;1,040</v>
@@ -2902,66 +3066,51 @@
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="72">
+      <c r="E6" s="56">
         <f>'ShareOfInflow-SEIS'!C15</f>
         <v>0.16401734104046239</v>
       </c>
-      <c r="H6" s="74" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" s="59">
-        <v>0.2107804750717828</v>
-      </c>
-      <c r="J6" s="59">
-        <v>0.25815713912816496</v>
-      </c>
-      <c r="K6" s="59">
-        <v>0.28817541111981204</v>
-      </c>
-      <c r="L6" s="59">
-        <v>0.75711302531975977</v>
-      </c>
-      <c r="M6" s="59">
-        <v>0.57426259462281393</v>
-      </c>
-      <c r="N6" s="59">
-        <v>0.52701644479248244</v>
-      </c>
-      <c r="O6" s="59">
-        <v>0.57426259462281393</v>
-      </c>
-      <c r="P6" s="59">
-        <v>1.6755416340381102</v>
-      </c>
-      <c r="Q6" s="59">
-        <v>0.18219785956669277</v>
-      </c>
-      <c r="R6" s="59">
-        <v>0.18219785956669277</v>
-      </c>
-      <c r="S6" s="59">
-        <v>0.18219785956669277</v>
-      </c>
-      <c r="T6" s="59">
-        <v>0.5465935787000783</v>
-      </c>
-      <c r="U6" s="59">
-        <v>3.2759070738710518E-2</v>
-      </c>
-      <c r="V6" s="59">
-        <v>3.2628556512659883E-2</v>
-      </c>
-      <c r="W6" s="59">
-        <v>3.5891412163925863E-2</v>
-      </c>
-      <c r="X6" s="59">
-        <v>0.10127903941529626</v>
-      </c>
-      <c r="Y6" s="59">
-        <v>3.0805272774732448</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="H6" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="76">
+        <v>0.29131652661064422</v>
+      </c>
+      <c r="J6" s="76">
+        <v>0.22625413801884389</v>
+      </c>
+      <c r="K6" s="76">
+        <v>0.26597911892029541</v>
+      </c>
+      <c r="L6" s="76">
+        <v>3.5523300229182576E-2</v>
+      </c>
+      <c r="M6" s="76">
+        <v>3.2722179781003308E-2</v>
+      </c>
+      <c r="N6" s="76">
+        <v>3.2849503437738729E-2</v>
+      </c>
+      <c r="O6" s="76">
+        <v>0.56022408963585435</v>
+      </c>
+      <c r="P6" s="76">
+        <v>0.56022408963585435</v>
+      </c>
+      <c r="Q6" s="76">
+        <v>0.52037178507766746</v>
+      </c>
+      <c r="R6" s="76">
+        <v>0.18079959256429842</v>
+      </c>
+      <c r="S6" s="76">
+        <v>0.18079959256429842</v>
+      </c>
+      <c r="T6" s="76">
+        <v>0.18079959256429842</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>'ShareOfInflow-SEIS'!A16</f>
         <v>1,040–&gt;1,035</v>
@@ -2977,66 +3126,51 @@
       <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="72">
+      <c r="E7" s="56">
         <f>'ShareOfInflow-SEIS'!C16</f>
         <v>0.15703090344521659</v>
       </c>
-      <c r="H7" s="74" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" s="59">
-        <v>0.15950735956743767</v>
-      </c>
-      <c r="J7" s="59">
-        <v>0.26119181737325819</v>
-      </c>
-      <c r="K7" s="59">
-        <v>0.31788079470198671</v>
-      </c>
-      <c r="L7" s="59">
-        <v>0.73857997164268263</v>
-      </c>
-      <c r="M7" s="59">
-        <v>0.60829077801141496</v>
-      </c>
-      <c r="N7" s="59">
-        <v>0.50770827156833676</v>
-      </c>
-      <c r="O7" s="59">
-        <v>0.59602649006622532</v>
-      </c>
-      <c r="P7" s="59">
-        <v>1.7120255396459771</v>
-      </c>
-      <c r="Q7" s="59">
-        <v>0.19960949234004208</v>
-      </c>
-      <c r="R7" s="59">
-        <v>0.19700563296768453</v>
-      </c>
-      <c r="S7" s="59">
-        <v>0.19558498896247239</v>
-      </c>
-      <c r="T7" s="59">
-        <v>0.59220011427019892</v>
-      </c>
-      <c r="U7" s="59">
-        <v>3.2592370081105437E-2</v>
-      </c>
-      <c r="V7" s="59">
-        <v>3.4094278090720423E-2</v>
-      </c>
-      <c r="W7" s="59">
-        <v>4.0176600441501099E-2</v>
-      </c>
-      <c r="X7" s="59">
-        <v>0.10686324861332697</v>
-      </c>
-      <c r="Y7" s="59">
-        <v>3.1496688741721859</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="H7" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="76">
+        <v>0.3033707865168539</v>
+      </c>
+      <c r="J7" s="76">
+        <v>0.16401734104046239</v>
+      </c>
+      <c r="K7" s="76">
+        <v>0.25786516853932584</v>
+      </c>
+      <c r="L7" s="76">
+        <v>3.8342696629213475E-2</v>
+      </c>
+      <c r="M7" s="76">
+        <v>3.3381502890173408E-2</v>
+      </c>
+      <c r="N7" s="76">
+        <v>3.3426966292134833E-2</v>
+      </c>
+      <c r="O7" s="76">
+        <v>0.5898876404494382</v>
+      </c>
+      <c r="P7" s="76">
+        <v>0.60693641618497118</v>
+      </c>
+      <c r="Q7" s="76">
+        <v>0.51839887640449445</v>
+      </c>
+      <c r="R7" s="76">
+        <v>0.19016853932584271</v>
+      </c>
+      <c r="S7" s="76">
+        <v>0.19566473988439309</v>
+      </c>
+      <c r="T7" s="76">
+        <v>0.19016853932584271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f>'ShareOfInflow-SEIS'!A17</f>
         <v>1,035–&gt;1,030</v>
@@ -3052,66 +3186,51 @@
       <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="72">
+      <c r="E8" s="56">
         <f>'ShareOfInflow-SEIS'!C17</f>
         <v>0.15810629745422058</v>
       </c>
-      <c r="H8" s="74" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" s="59">
-        <v>0.15810629745422058</v>
-      </c>
-      <c r="J8" s="59">
-        <v>0.25803108808290154</v>
-      </c>
-      <c r="K8" s="59">
-        <v>0.31286210892236382</v>
-      </c>
-      <c r="L8" s="59">
-        <v>0.72899949445948597</v>
-      </c>
-      <c r="M8" s="59">
-        <v>0.61039154384397798</v>
-      </c>
-      <c r="N8" s="59">
-        <v>0.50999259807549968</v>
-      </c>
-      <c r="O8" s="59">
-        <v>0.59385863267670924</v>
-      </c>
-      <c r="P8" s="59">
-        <v>1.7142427745961868</v>
-      </c>
-      <c r="Q8" s="59">
-        <v>0.19919606967396158</v>
-      </c>
-      <c r="R8" s="59">
-        <v>0.19807549962990378</v>
-      </c>
-      <c r="S8" s="59">
-        <v>0.19380069524913096</v>
-      </c>
-      <c r="T8" s="59">
-        <v>0.59107226455299633</v>
-      </c>
-      <c r="U8" s="59">
-        <v>3.2306089027839803E-2</v>
-      </c>
-      <c r="V8" s="59">
-        <v>3.3752775721687639E-2</v>
-      </c>
-      <c r="W8" s="59">
-        <v>3.9542294322132091E-2</v>
-      </c>
-      <c r="X8" s="59">
-        <v>0.10560115907165953</v>
-      </c>
-      <c r="Y8" s="59">
-        <v>3.1399156926803289</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="H8" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="76">
+        <v>0.30804335424985735</v>
+      </c>
+      <c r="J8" s="76">
+        <v>0.15703090344521659</v>
+      </c>
+      <c r="K8" s="76">
+        <v>0.25506432056779532</v>
+      </c>
+      <c r="L8" s="76">
+        <v>3.8933257273245855E-2</v>
+      </c>
+      <c r="M8" s="76">
+        <v>3.2086352210557438E-2</v>
+      </c>
+      <c r="N8" s="76">
+        <v>3.3417122578737246E-2</v>
+      </c>
+      <c r="O8" s="76">
+        <v>0.59184255561893895</v>
+      </c>
+      <c r="P8" s="76">
+        <v>0.6118586426142244</v>
+      </c>
+      <c r="Q8" s="76">
+        <v>0.51249445512346592</v>
+      </c>
+      <c r="R8" s="76">
+        <v>0.19195664575014262</v>
+      </c>
+      <c r="S8" s="76">
+        <v>0.19902410173000148</v>
+      </c>
+      <c r="T8" s="76">
+        <v>0.19902410173000148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>'ShareOfInflow-SEIS'!A18</f>
         <v>1,030–1,025</v>
@@ -3127,66 +3246,51 @@
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="72">
+      <c r="E9" s="56">
         <f>'ShareOfInflow-SEIS'!C18</f>
         <v>0.15950735956743767</v>
       </c>
-      <c r="H9" s="74" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="59">
-        <v>0.15703090344521659</v>
-      </c>
-      <c r="J9" s="59">
-        <v>0.25506432056779532</v>
-      </c>
-      <c r="K9" s="59">
-        <v>0.30804335424985735</v>
-      </c>
-      <c r="L9" s="59">
-        <v>0.72013857826286931</v>
-      </c>
-      <c r="M9" s="59">
-        <v>0.6118586426142244</v>
-      </c>
-      <c r="N9" s="59">
-        <v>0.51249445512346592</v>
-      </c>
-      <c r="O9" s="59">
-        <v>0.59184255561893895</v>
-      </c>
-      <c r="P9" s="59">
-        <v>1.7161956533566292</v>
-      </c>
-      <c r="Q9" s="59">
-        <v>0.19902410173000148</v>
-      </c>
-      <c r="R9" s="59">
-        <v>0.19902410173000148</v>
-      </c>
-      <c r="S9" s="59">
-        <v>0.19195664575014262</v>
-      </c>
-      <c r="T9" s="59">
-        <v>0.59000484921014562</v>
-      </c>
-      <c r="U9" s="59">
-        <v>3.2086352210557438E-2</v>
-      </c>
-      <c r="V9" s="59">
-        <v>3.3417122578737246E-2</v>
-      </c>
-      <c r="W9" s="59">
-        <v>3.8933257273245855E-2</v>
-      </c>
-      <c r="X9" s="59">
-        <v>0.10443673206254055</v>
-      </c>
-      <c r="Y9" s="59">
-        <v>3.1307758128921845</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="H9" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="76">
+        <v>0.31286210892236382</v>
+      </c>
+      <c r="J9" s="76">
+        <v>0.15810629745422058</v>
+      </c>
+      <c r="K9" s="76">
+        <v>0.25803108808290154</v>
+      </c>
+      <c r="L9" s="76">
+        <v>3.9542294322132091E-2</v>
+      </c>
+      <c r="M9" s="76">
+        <v>3.2306089027839803E-2</v>
+      </c>
+      <c r="N9" s="76">
+        <v>3.3752775721687639E-2</v>
+      </c>
+      <c r="O9" s="76">
+        <v>0.59385863267670924</v>
+      </c>
+      <c r="P9" s="76">
+        <v>0.61039154384397798</v>
+      </c>
+      <c r="Q9" s="76">
+        <v>0.50999259807549968</v>
+      </c>
+      <c r="R9" s="76">
+        <v>0.19380069524913096</v>
+      </c>
+      <c r="S9" s="76">
+        <v>0.19919606967396158</v>
+      </c>
+      <c r="T9" s="76">
+        <v>0.19807549962990378</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f>'ShareOfInflow-SEIS'!A19</f>
         <v>&lt;1,025–1,000</v>
@@ -3202,66 +3306,51 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="72">
+      <c r="E10" s="56">
         <f>'ShareOfInflow-SEIS'!C19</f>
         <v>0.1620384498016478</v>
       </c>
-      <c r="H10" s="74" t="s">
-        <v>52</v>
-      </c>
-      <c r="I10" s="59">
-        <v>0.16401734104046239</v>
-      </c>
-      <c r="J10" s="59">
-        <v>0.25786516853932584</v>
-      </c>
-      <c r="K10" s="59">
-        <v>0.3033707865168539</v>
-      </c>
-      <c r="L10" s="59">
-        <v>0.72525329609664213</v>
-      </c>
-      <c r="M10" s="59">
-        <v>0.60693641618497118</v>
-      </c>
-      <c r="N10" s="59">
-        <v>0.51839887640449445</v>
-      </c>
-      <c r="O10" s="59">
-        <v>0.5898876404494382</v>
-      </c>
-      <c r="P10" s="59">
-        <v>1.7152229330389039</v>
-      </c>
-      <c r="Q10" s="59">
-        <v>0.19566473988439309</v>
-      </c>
-      <c r="R10" s="59">
-        <v>0.19016853932584271</v>
-      </c>
-      <c r="S10" s="59">
-        <v>0.19016853932584271</v>
-      </c>
-      <c r="T10" s="59">
-        <v>0.57600181853607846</v>
-      </c>
-      <c r="U10" s="59">
-        <v>3.3381502890173408E-2</v>
-      </c>
-      <c r="V10" s="59">
-        <v>3.3426966292134833E-2</v>
-      </c>
-      <c r="W10" s="59">
-        <v>3.8342696629213475E-2</v>
-      </c>
-      <c r="X10" s="59">
-        <v>0.1051511658115217</v>
-      </c>
-      <c r="Y10" s="59">
-        <v>3.1216292134831458</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="H10" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="76">
+        <v>0.31788079470198671</v>
+      </c>
+      <c r="J10" s="76">
+        <v>0.15950735956743767</v>
+      </c>
+      <c r="K10" s="76">
+        <v>0.26119181737325819</v>
+      </c>
+      <c r="L10" s="76">
+        <v>4.0176600441501099E-2</v>
+      </c>
+      <c r="M10" s="76">
+        <v>3.2592370081105437E-2</v>
+      </c>
+      <c r="N10" s="76">
+        <v>3.4094278090720423E-2</v>
+      </c>
+      <c r="O10" s="76">
+        <v>0.59602649006622532</v>
+      </c>
+      <c r="P10" s="76">
+        <v>0.60829077801141496</v>
+      </c>
+      <c r="Q10" s="76">
+        <v>0.50770827156833676</v>
+      </c>
+      <c r="R10" s="76">
+        <v>0.19558498896247239</v>
+      </c>
+      <c r="S10" s="76">
+        <v>0.19960949234004208</v>
+      </c>
+      <c r="T10" s="76">
+        <v>0.19700563296768453</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>A3</f>
         <v>1,090–&gt;1,075</v>
@@ -3278,66 +3367,51 @@
         <f>D3</f>
         <v>Arizona</v>
       </c>
-      <c r="E11" s="72">
+      <c r="E11" s="56">
         <f>'ShareOfInflow-SEIS'!H12</f>
         <v>0.29594578805935273</v>
       </c>
-      <c r="H11" s="74" t="s">
-        <v>50</v>
-      </c>
-      <c r="I11" s="59">
-        <v>0.22625413801884389</v>
-      </c>
-      <c r="J11" s="59">
-        <v>0.26597911892029541</v>
-      </c>
-      <c r="K11" s="59">
-        <v>0.29131652661064422</v>
-      </c>
-      <c r="L11" s="59">
-        <v>0.78354978354978355</v>
-      </c>
-      <c r="M11" s="59">
-        <v>0.56022408963585435</v>
-      </c>
-      <c r="N11" s="59">
-        <v>0.52037178507766746</v>
-      </c>
-      <c r="O11" s="59">
-        <v>0.56022408963585435</v>
-      </c>
-      <c r="P11" s="59">
-        <v>1.6408199643493762</v>
-      </c>
-      <c r="Q11" s="59">
-        <v>0.18079959256429842</v>
-      </c>
-      <c r="R11" s="59">
-        <v>0.18079959256429842</v>
-      </c>
-      <c r="S11" s="59">
-        <v>0.18079959256429842</v>
-      </c>
-      <c r="T11" s="59">
-        <v>0.54239877769289524</v>
-      </c>
-      <c r="U11" s="59">
-        <v>3.2722179781003308E-2</v>
-      </c>
-      <c r="V11" s="59">
-        <v>3.2849503437738729E-2</v>
-      </c>
-      <c r="W11" s="59">
-        <v>3.5523300229182576E-2</v>
-      </c>
-      <c r="X11" s="59">
-        <v>0.10109498344792461</v>
-      </c>
-      <c r="Y11" s="59">
-        <v>3.0678635090399795</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="H11" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="76">
+        <v>0.28817541111981204</v>
+      </c>
+      <c r="J11" s="76">
+        <v>0.2107804750717828</v>
+      </c>
+      <c r="K11" s="76">
+        <v>0.25815713912816496</v>
+      </c>
+      <c r="L11" s="76">
+        <v>3.5891412163925863E-2</v>
+      </c>
+      <c r="M11" s="76">
+        <v>3.2759070738710518E-2</v>
+      </c>
+      <c r="N11" s="76">
+        <v>3.2628556512659883E-2</v>
+      </c>
+      <c r="O11" s="76">
+        <v>0.57426259462281393</v>
+      </c>
+      <c r="P11" s="76">
+        <v>0.57426259462281393</v>
+      </c>
+      <c r="Q11" s="76">
+        <v>0.52701644479248244</v>
+      </c>
+      <c r="R11" s="76">
+        <v>0.18219785956669277</v>
+      </c>
+      <c r="S11" s="76">
+        <v>0.18219785956669277</v>
+      </c>
+      <c r="T11" s="76">
+        <v>0.18219785956669277</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f t="shared" ref="A12:B12" si="0">A4</f>
         <v>1,075–1,050</v>
@@ -3354,66 +3428,51 @@
         <f t="shared" ref="D12:D26" si="1">D4</f>
         <v>Arizona</v>
       </c>
-      <c r="E12" s="72">
+      <c r="E12" s="56">
         <f>'ShareOfInflow-SEIS'!H13</f>
         <v>0.26597911892029541</v>
       </c>
-      <c r="H12" s="74" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" s="59">
-        <v>0.2822759668185536</v>
-      </c>
-      <c r="J12" s="59">
-        <v>0.29594578805935273</v>
-      </c>
-      <c r="K12" s="59">
-        <v>0.30470849398294192</v>
-      </c>
-      <c r="L12" s="59">
-        <v>0.88293024886084814</v>
-      </c>
-      <c r="M12" s="59">
-        <v>0.51407874751723337</v>
-      </c>
-      <c r="N12" s="59">
-        <v>0.5004089262764343</v>
-      </c>
-      <c r="O12" s="59">
-        <v>0.51407874751723337</v>
-      </c>
-      <c r="P12" s="59">
-        <v>1.5285664213109009</v>
-      </c>
-      <c r="Q12" s="59">
-        <v>0.17046383923355535</v>
-      </c>
-      <c r="R12" s="59">
-        <v>0.17046383923355535</v>
-      </c>
-      <c r="S12" s="59">
-        <v>0.17046383923355535</v>
-      </c>
-      <c r="T12" s="59">
-        <v>0.51139151770066604</v>
-      </c>
-      <c r="U12" s="59">
-        <v>3.3181446430657784E-2</v>
-      </c>
-      <c r="V12" s="59">
-        <v>3.3181446430657784E-2</v>
-      </c>
-      <c r="W12" s="59">
-        <v>3.4116135062507304E-2</v>
-      </c>
-      <c r="X12" s="59">
-        <v>0.10047902792382288</v>
-      </c>
-      <c r="Y12" s="59">
-        <v>3.0233672157962381</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="H12" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="76">
+        <v>0.31877394636015327</v>
+      </c>
+      <c r="J12" s="76">
+        <v>0.1620384498016478</v>
+      </c>
+      <c r="K12" s="76">
+        <v>0.25790424570912374</v>
+      </c>
+      <c r="L12" s="76">
+        <v>4.1379310344827586E-2</v>
+      </c>
+      <c r="M12" s="76">
+        <v>3.3109551418980768E-2</v>
+      </c>
+      <c r="N12" s="76">
+        <v>3.4778681120144532E-2</v>
+      </c>
+      <c r="O12" s="76">
+        <v>0.62068965517241392</v>
+      </c>
+      <c r="P12" s="76">
+        <v>0.61794324076899609</v>
+      </c>
+      <c r="Q12" s="76">
+        <v>0.52288467329117749</v>
+      </c>
+      <c r="R12" s="76">
+        <v>0.18773946360153257</v>
+      </c>
+      <c r="S12" s="76">
+        <v>0.18690875801037535</v>
+      </c>
+      <c r="T12" s="76">
+        <v>0.18443239987955437</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f t="shared" ref="A13:B13" si="2">A5</f>
         <v>&lt;1,050–&gt;1,045</v>
@@ -3430,66 +3489,12 @@
         <f t="shared" si="1"/>
         <v>Arizona</v>
       </c>
-      <c r="E13" s="72">
+      <c r="E13" s="56">
         <f>'ShareOfInflow-SEIS'!H14</f>
         <v>0.25815713912816496</v>
       </c>
-      <c r="H13" s="74" t="s">
-        <v>92</v>
-      </c>
-      <c r="I13" s="59">
-        <v>1.5200109312181653</v>
-      </c>
-      <c r="J13" s="59">
-        <v>2.1101386863802176</v>
-      </c>
-      <c r="K13" s="59">
-        <v>2.445131422464613</v>
-      </c>
-      <c r="L13" s="59">
-        <v>6.0752810400629951</v>
-      </c>
-      <c r="M13" s="59">
-        <v>4.7039860531994862</v>
-      </c>
-      <c r="N13" s="59">
-        <v>4.1192760306095586</v>
-      </c>
-      <c r="O13" s="59">
-        <v>4.6408704057596273</v>
-      </c>
-      <c r="P13" s="59">
-        <v>13.464132489568671</v>
-      </c>
-      <c r="Q13" s="59">
-        <v>1.5138644530033201</v>
-      </c>
-      <c r="R13" s="59">
-        <v>1.5021674648975336</v>
-      </c>
-      <c r="S13" s="59">
-        <v>1.4927116242536678</v>
-      </c>
-      <c r="T13" s="59">
-        <v>4.5087435421545212</v>
-      </c>
-      <c r="U13" s="59">
-        <v>0.26213856257902846</v>
-      </c>
-      <c r="V13" s="59">
-        <v>0.2681293301844811</v>
-      </c>
-      <c r="W13" s="59">
-        <v>0.3039050064665359</v>
-      </c>
-      <c r="X13" s="59">
-        <v>0.83417289923004534</v>
-      </c>
-      <c r="Y13" s="59">
-        <v>24.882329971016237</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
         <f t="shared" ref="A14:B14" si="3">A6</f>
         <v>1,045–&gt;1,040</v>
@@ -3506,12 +3511,12 @@
         <f t="shared" si="1"/>
         <v>Arizona</v>
       </c>
-      <c r="E14" s="72">
+      <c r="E14" s="56">
         <f>'ShareOfInflow-SEIS'!H15</f>
         <v>0.25786516853932584</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
         <f t="shared" ref="A15:B15" si="4">A7</f>
         <v>1,040–&gt;1,035</v>
@@ -3528,12 +3533,12 @@
         <f t="shared" si="1"/>
         <v>Arizona</v>
       </c>
-      <c r="E15" s="72">
+      <c r="E15" s="56">
         <f>'ShareOfInflow-SEIS'!H16</f>
         <v>0.25506432056779532</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f t="shared" ref="A16:B16" si="5">A8</f>
         <v>1,035–&gt;1,030</v>
@@ -3550,7 +3555,7 @@
         <f t="shared" si="1"/>
         <v>Arizona</v>
       </c>
-      <c r="E16" s="72">
+      <c r="E16" s="56">
         <f>'ShareOfInflow-SEIS'!H17</f>
         <v>0.25803108808290154</v>
       </c>
@@ -3572,7 +3577,7 @@
         <f t="shared" si="1"/>
         <v>Arizona</v>
       </c>
-      <c r="E17" s="72">
+      <c r="E17" s="56">
         <f>'ShareOfInflow-SEIS'!H18</f>
         <v>0.26119181737325819</v>
       </c>
@@ -3594,7 +3599,7 @@
         <f t="shared" si="1"/>
         <v>Arizona</v>
       </c>
-      <c r="E18" s="72">
+      <c r="E18" s="56">
         <f>'ShareOfInflow-SEIS'!H19</f>
         <v>0.25790424570912374</v>
       </c>
@@ -3616,7 +3621,7 @@
         <f>D11</f>
         <v>Arizona</v>
       </c>
-      <c r="E19" s="72">
+      <c r="E19" s="56">
         <f>'ShareOfInflow-SEIS'!M12</f>
         <v>0.30470849398294192</v>
       </c>
@@ -3638,7 +3643,7 @@
         <f t="shared" si="1"/>
         <v>Arizona</v>
       </c>
-      <c r="E20" s="72">
+      <c r="E20" s="56">
         <f>'ShareOfInflow-SEIS'!M13</f>
         <v>0.29131652661064422</v>
       </c>
@@ -3660,7 +3665,7 @@
         <f t="shared" si="1"/>
         <v>Arizona</v>
       </c>
-      <c r="E21" s="72">
+      <c r="E21" s="56">
         <f>'ShareOfInflow-SEIS'!M14</f>
         <v>0.28817541111981204</v>
       </c>
@@ -3682,7 +3687,7 @@
         <f t="shared" si="1"/>
         <v>Arizona</v>
       </c>
-      <c r="E22" s="72">
+      <c r="E22" s="56">
         <f>'ShareOfInflow-SEIS'!M15</f>
         <v>0.3033707865168539</v>
       </c>
@@ -3704,7 +3709,7 @@
         <f t="shared" si="1"/>
         <v>Arizona</v>
       </c>
-      <c r="E23" s="72">
+      <c r="E23" s="56">
         <f>'ShareOfInflow-SEIS'!M16</f>
         <v>0.30804335424985735</v>
       </c>
@@ -3726,7 +3731,7 @@
         <f t="shared" si="1"/>
         <v>Arizona</v>
       </c>
-      <c r="E24" s="72">
+      <c r="E24" s="56">
         <f>'ShareOfInflow-SEIS'!M17</f>
         <v>0.31286210892236382</v>
       </c>
@@ -3748,7 +3753,7 @@
         <f t="shared" si="1"/>
         <v>Arizona</v>
       </c>
-      <c r="E25" s="72">
+      <c r="E25" s="56">
         <f>'ShareOfInflow-SEIS'!M18</f>
         <v>0.31788079470198671</v>
       </c>
@@ -3770,7 +3775,7 @@
         <f t="shared" si="1"/>
         <v>Arizona</v>
       </c>
-      <c r="E26" s="72">
+      <c r="E26" s="56">
         <f>'ShareOfInflow-SEIS'!M19</f>
         <v>0.31877394636015327</v>
       </c>
@@ -3791,7 +3796,7 @@
       <c r="D27" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="72">
+      <c r="E27" s="56">
         <f>'ShareOfInflow-SEIS'!D12</f>
         <v>3.3181446430657784E-2</v>
       </c>
@@ -3812,7 +3817,7 @@
       <c r="D28" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="72">
+      <c r="E28" s="56">
         <f>'ShareOfInflow-SEIS'!D13</f>
         <v>3.2722179781003308E-2</v>
       </c>
@@ -3833,7 +3838,7 @@
       <c r="D29" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="72">
+      <c r="E29" s="56">
         <f>'ShareOfInflow-SEIS'!D14</f>
         <v>3.2759070738710518E-2</v>
       </c>
@@ -3854,7 +3859,7 @@
       <c r="D30" t="s">
         <v>19</v>
       </c>
-      <c r="E30" s="72">
+      <c r="E30" s="56">
         <f>'ShareOfInflow-SEIS'!D15</f>
         <v>3.3381502890173408E-2</v>
       </c>
@@ -3875,7 +3880,7 @@
       <c r="D31" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="72">
+      <c r="E31" s="56">
         <f>'ShareOfInflow-SEIS'!D16</f>
         <v>3.2086352210557438E-2</v>
       </c>
@@ -3896,7 +3901,7 @@
       <c r="D32" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="72">
+      <c r="E32" s="56">
         <f>'ShareOfInflow-SEIS'!D17</f>
         <v>3.2306089027839803E-2</v>
       </c>
@@ -3917,7 +3922,7 @@
       <c r="D33" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="72">
+      <c r="E33" s="56">
         <f>'ShareOfInflow-SEIS'!D18</f>
         <v>3.2592370081105437E-2</v>
       </c>
@@ -3938,7 +3943,7 @@
       <c r="D34" t="s">
         <v>19</v>
       </c>
-      <c r="E34" s="72">
+      <c r="E34" s="56">
         <f>'ShareOfInflow-SEIS'!D19</f>
         <v>3.3109551418980768E-2</v>
       </c>
@@ -3959,7 +3964,7 @@
       <c r="D35" t="s">
         <v>19</v>
       </c>
-      <c r="E35" s="72">
+      <c r="E35" s="56">
         <f>'ShareOfInflow-SEIS'!I12</f>
         <v>3.3181446430657784E-2</v>
       </c>
@@ -3980,7 +3985,7 @@
       <c r="D36" t="s">
         <v>19</v>
       </c>
-      <c r="E36" s="72">
+      <c r="E36" s="56">
         <f>'ShareOfInflow-SEIS'!I13</f>
         <v>3.2849503437738729E-2</v>
       </c>
@@ -4001,7 +4006,7 @@
       <c r="D37" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="72">
+      <c r="E37" s="56">
         <f>'ShareOfInflow-SEIS'!I14</f>
         <v>3.2628556512659883E-2</v>
       </c>
@@ -4022,7 +4027,7 @@
       <c r="D38" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="72">
+      <c r="E38" s="56">
         <f>'ShareOfInflow-SEIS'!I15</f>
         <v>3.3426966292134833E-2</v>
       </c>
@@ -4043,7 +4048,7 @@
       <c r="D39" t="s">
         <v>19</v>
       </c>
-      <c r="E39" s="72">
+      <c r="E39" s="56">
         <f>'ShareOfInflow-SEIS'!I16</f>
         <v>3.3417122578737246E-2</v>
       </c>
@@ -4064,7 +4069,7 @@
       <c r="D40" t="s">
         <v>19</v>
       </c>
-      <c r="E40" s="72">
+      <c r="E40" s="56">
         <f>'ShareOfInflow-SEIS'!I17</f>
         <v>3.3752775721687639E-2</v>
       </c>
@@ -4085,7 +4090,7 @@
       <c r="D41" t="s">
         <v>19</v>
       </c>
-      <c r="E41" s="72">
+      <c r="E41" s="56">
         <f>'ShareOfInflow-SEIS'!I18</f>
         <v>3.4094278090720423E-2</v>
       </c>
@@ -4106,7 +4111,7 @@
       <c r="D42" t="s">
         <v>19</v>
       </c>
-      <c r="E42" s="72">
+      <c r="E42" s="56">
         <f>'ShareOfInflow-SEIS'!I19</f>
         <v>3.4778681120144532E-2</v>
       </c>
@@ -4127,7 +4132,7 @@
       <c r="D43" t="s">
         <v>19</v>
       </c>
-      <c r="E43" s="72">
+      <c r="E43" s="56">
         <f>'ShareOfInflow-SEIS'!N12</f>
         <v>3.4116135062507304E-2</v>
       </c>
@@ -4148,7 +4153,7 @@
       <c r="D44" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="72">
+      <c r="E44" s="56">
         <f>'ShareOfInflow-SEIS'!N13</f>
         <v>3.5523300229182576E-2</v>
       </c>
@@ -4169,7 +4174,7 @@
       <c r="D45" t="s">
         <v>19</v>
       </c>
-      <c r="E45" s="72">
+      <c r="E45" s="56">
         <f>'ShareOfInflow-SEIS'!N14</f>
         <v>3.5891412163925863E-2</v>
       </c>
@@ -4190,7 +4195,7 @@
       <c r="D46" t="s">
         <v>19</v>
       </c>
-      <c r="E46" s="72">
+      <c r="E46" s="56">
         <f>'ShareOfInflow-SEIS'!N15</f>
         <v>3.8342696629213475E-2</v>
       </c>
@@ -4211,7 +4216,7 @@
       <c r="D47" t="s">
         <v>19</v>
       </c>
-      <c r="E47" s="72">
+      <c r="E47" s="56">
         <f>'ShareOfInflow-SEIS'!N16</f>
         <v>3.8933257273245855E-2</v>
       </c>
@@ -4232,7 +4237,7 @@
       <c r="D48" t="s">
         <v>19</v>
       </c>
-      <c r="E48" s="72">
+      <c r="E48" s="56">
         <f>'ShareOfInflow-SEIS'!N17</f>
         <v>3.9542294322132091E-2</v>
       </c>
@@ -4253,7 +4258,7 @@
       <c r="D49" t="s">
         <v>19</v>
       </c>
-      <c r="E49" s="72">
+      <c r="E49" s="56">
         <f>'ShareOfInflow-SEIS'!N18</f>
         <v>4.0176600441501099E-2</v>
       </c>
@@ -4274,7 +4279,7 @@
       <c r="D50" t="s">
         <v>19</v>
       </c>
-      <c r="E50" s="72">
+      <c r="E50" s="56">
         <f>'ShareOfInflow-SEIS'!N19</f>
         <v>4.1379310344827586E-2</v>
       </c>
@@ -4295,7 +4300,7 @@
       <c r="D51" t="s">
         <v>20</v>
       </c>
-      <c r="E51" s="72">
+      <c r="E51" s="56">
         <f>'ShareOfInflow-SEIS'!E12</f>
         <v>0.51407874751723337</v>
       </c>
@@ -4316,7 +4321,7 @@
       <c r="D52" t="s">
         <v>20</v>
       </c>
-      <c r="E52" s="72">
+      <c r="E52" s="56">
         <f>'ShareOfInflow-SEIS'!E13</f>
         <v>0.56022408963585435</v>
       </c>
@@ -4337,7 +4342,7 @@
       <c r="D53" t="s">
         <v>20</v>
       </c>
-      <c r="E53" s="72">
+      <c r="E53" s="56">
         <f>'ShareOfInflow-SEIS'!E14</f>
         <v>0.57426259462281393</v>
       </c>
@@ -4358,7 +4363,7 @@
       <c r="D54" t="s">
         <v>20</v>
       </c>
-      <c r="E54" s="72">
+      <c r="E54" s="56">
         <f>'ShareOfInflow-SEIS'!E15</f>
         <v>0.60693641618497118</v>
       </c>
@@ -4379,7 +4384,7 @@
       <c r="D55" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="72">
+      <c r="E55" s="56">
         <f>'ShareOfInflow-SEIS'!E16</f>
         <v>0.6118586426142244</v>
       </c>
@@ -4400,7 +4405,7 @@
       <c r="D56" t="s">
         <v>20</v>
       </c>
-      <c r="E56" s="72">
+      <c r="E56" s="56">
         <f>'ShareOfInflow-SEIS'!E17</f>
         <v>0.61039154384397798</v>
       </c>
@@ -4421,7 +4426,7 @@
       <c r="D57" t="s">
         <v>20</v>
       </c>
-      <c r="E57" s="72">
+      <c r="E57" s="56">
         <f>'ShareOfInflow-SEIS'!E18</f>
         <v>0.60829077801141496</v>
       </c>
@@ -4442,7 +4447,7 @@
       <c r="D58" t="s">
         <v>20</v>
       </c>
-      <c r="E58" s="72">
+      <c r="E58" s="56">
         <f>'ShareOfInflow-SEIS'!E19</f>
         <v>0.61794324076899609</v>
       </c>
@@ -4463,7 +4468,7 @@
       <c r="D59" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="72">
+      <c r="E59" s="56">
         <f>'ShareOfInflow-SEIS'!J12</f>
         <v>0.5004089262764343</v>
       </c>
@@ -4484,7 +4489,7 @@
       <c r="D60" t="s">
         <v>20</v>
       </c>
-      <c r="E60" s="72">
+      <c r="E60" s="56">
         <f>'ShareOfInflow-SEIS'!J13</f>
         <v>0.52037178507766746</v>
       </c>
@@ -4505,7 +4510,7 @@
       <c r="D61" t="s">
         <v>20</v>
       </c>
-      <c r="E61" s="72">
+      <c r="E61" s="56">
         <f>'ShareOfInflow-SEIS'!J14</f>
         <v>0.52701644479248244</v>
       </c>
@@ -4526,7 +4531,7 @@
       <c r="D62" t="s">
         <v>20</v>
       </c>
-      <c r="E62" s="72">
+      <c r="E62" s="56">
         <f>'ShareOfInflow-SEIS'!J15</f>
         <v>0.51839887640449445</v>
       </c>
@@ -4547,7 +4552,7 @@
       <c r="D63" t="s">
         <v>20</v>
       </c>
-      <c r="E63" s="72">
+      <c r="E63" s="56">
         <f>'ShareOfInflow-SEIS'!J16</f>
         <v>0.51249445512346592</v>
       </c>
@@ -4568,7 +4573,7 @@
       <c r="D64" t="s">
         <v>20</v>
       </c>
-      <c r="E64" s="72">
+      <c r="E64" s="56">
         <f>'ShareOfInflow-SEIS'!J17</f>
         <v>0.50999259807549968</v>
       </c>
@@ -4589,7 +4594,7 @@
       <c r="D65" t="s">
         <v>20</v>
       </c>
-      <c r="E65" s="72">
+      <c r="E65" s="56">
         <f>'ShareOfInflow-SEIS'!J18</f>
         <v>0.50770827156833676</v>
       </c>
@@ -4610,7 +4615,7 @@
       <c r="D66" t="s">
         <v>20</v>
       </c>
-      <c r="E66" s="72">
+      <c r="E66" s="56">
         <f>'ShareOfInflow-SEIS'!J19</f>
         <v>0.52288467329117749</v>
       </c>
@@ -4631,7 +4636,7 @@
       <c r="D67" t="s">
         <v>20</v>
       </c>
-      <c r="E67" s="72">
+      <c r="E67" s="56">
         <f>'ShareOfInflow-SEIS'!O12</f>
         <v>0.51407874751723337</v>
       </c>
@@ -4652,7 +4657,7 @@
       <c r="D68" t="s">
         <v>20</v>
       </c>
-      <c r="E68" s="72">
+      <c r="E68" s="56">
         <f>'ShareOfInflow-SEIS'!O13</f>
         <v>0.56022408963585435</v>
       </c>
@@ -4673,7 +4678,7 @@
       <c r="D69" t="s">
         <v>20</v>
       </c>
-      <c r="E69" s="72">
+      <c r="E69" s="56">
         <f>'ShareOfInflow-SEIS'!O14</f>
         <v>0.57426259462281393</v>
       </c>
@@ -4694,7 +4699,7 @@
       <c r="D70" t="s">
         <v>20</v>
       </c>
-      <c r="E70" s="72">
+      <c r="E70" s="56">
         <f>'ShareOfInflow-SEIS'!O15</f>
         <v>0.5898876404494382</v>
       </c>
@@ -4715,7 +4720,7 @@
       <c r="D71" t="s">
         <v>20</v>
       </c>
-      <c r="E71" s="72">
+      <c r="E71" s="56">
         <f>'ShareOfInflow-SEIS'!O16</f>
         <v>0.59184255561893895</v>
       </c>
@@ -4736,7 +4741,7 @@
       <c r="D72" t="s">
         <v>20</v>
       </c>
-      <c r="E72" s="72">
+      <c r="E72" s="56">
         <f>'ShareOfInflow-SEIS'!O17</f>
         <v>0.59385863267670924</v>
       </c>
@@ -4757,7 +4762,7 @@
       <c r="D73" t="s">
         <v>20</v>
       </c>
-      <c r="E73" s="72">
+      <c r="E73" s="56">
         <f>'ShareOfInflow-SEIS'!O18</f>
         <v>0.59602649006622532</v>
       </c>
@@ -4778,7 +4783,7 @@
       <c r="D74" t="s">
         <v>20</v>
       </c>
-      <c r="E74" s="72">
+      <c r="E74" s="56">
         <f>'ShareOfInflow-SEIS'!O19</f>
         <v>0.62068965517241392</v>
       </c>
@@ -4799,7 +4804,7 @@
       <c r="D75" t="s">
         <v>4</v>
       </c>
-      <c r="E75" s="72">
+      <c r="E75" s="56">
         <f>'ShareOfInflow-SEIS'!F12</f>
         <v>0.17046383923355535</v>
       </c>
@@ -4820,7 +4825,7 @@
       <c r="D76" t="s">
         <v>4</v>
       </c>
-      <c r="E76" s="72">
+      <c r="E76" s="56">
         <f>'ShareOfInflow-SEIS'!F13</f>
         <v>0.18079959256429842</v>
       </c>
@@ -4841,7 +4846,7 @@
       <c r="D77" t="s">
         <v>4</v>
       </c>
-      <c r="E77" s="72">
+      <c r="E77" s="56">
         <f>'ShareOfInflow-SEIS'!F14</f>
         <v>0.18219785956669277</v>
       </c>
@@ -4862,7 +4867,7 @@
       <c r="D78" t="s">
         <v>4</v>
       </c>
-      <c r="E78" s="72">
+      <c r="E78" s="56">
         <f>'ShareOfInflow-SEIS'!F15</f>
         <v>0.19566473988439309</v>
       </c>
@@ -4883,7 +4888,7 @@
       <c r="D79" t="s">
         <v>4</v>
       </c>
-      <c r="E79" s="72">
+      <c r="E79" s="56">
         <f>'ShareOfInflow-SEIS'!F16</f>
         <v>0.19902410173000148</v>
       </c>
@@ -4904,7 +4909,7 @@
       <c r="D80" t="s">
         <v>4</v>
       </c>
-      <c r="E80" s="72">
+      <c r="E80" s="56">
         <f>'ShareOfInflow-SEIS'!F17</f>
         <v>0.19919606967396158</v>
       </c>
@@ -4925,7 +4930,7 @@
       <c r="D81" t="s">
         <v>4</v>
       </c>
-      <c r="E81" s="72">
+      <c r="E81" s="56">
         <f>'ShareOfInflow-SEIS'!F18</f>
         <v>0.19960949234004208</v>
       </c>
@@ -4946,7 +4951,7 @@
       <c r="D82" t="s">
         <v>4</v>
       </c>
-      <c r="E82" s="72">
+      <c r="E82" s="56">
         <f>'ShareOfInflow-SEIS'!F19</f>
         <v>0.18690875801037535</v>
       </c>
@@ -4967,7 +4972,7 @@
       <c r="D83" t="s">
         <v>4</v>
       </c>
-      <c r="E83" s="72">
+      <c r="E83" s="56">
         <f>'ShareOfInflow-SEIS'!K12</f>
         <v>0.17046383923355535</v>
       </c>
@@ -4988,7 +4993,7 @@
       <c r="D84" t="s">
         <v>4</v>
       </c>
-      <c r="E84" s="72">
+      <c r="E84" s="56">
         <f>'ShareOfInflow-SEIS'!K13</f>
         <v>0.18079959256429842</v>
       </c>
@@ -5009,7 +5014,7 @@
       <c r="D85" t="s">
         <v>4</v>
       </c>
-      <c r="E85" s="72">
+      <c r="E85" s="56">
         <f>'ShareOfInflow-SEIS'!K14</f>
         <v>0.18219785956669277</v>
       </c>
@@ -5030,7 +5035,7 @@
       <c r="D86" t="s">
         <v>4</v>
       </c>
-      <c r="E86" s="72">
+      <c r="E86" s="56">
         <f>'ShareOfInflow-SEIS'!K15</f>
         <v>0.19016853932584271</v>
       </c>
@@ -5051,7 +5056,7 @@
       <c r="D87" t="s">
         <v>4</v>
       </c>
-      <c r="E87" s="72">
+      <c r="E87" s="56">
         <f>'ShareOfInflow-SEIS'!K16</f>
         <v>0.19902410173000148</v>
       </c>
@@ -5072,7 +5077,7 @@
       <c r="D88" t="s">
         <v>4</v>
       </c>
-      <c r="E88" s="72">
+      <c r="E88" s="56">
         <f>'ShareOfInflow-SEIS'!K17</f>
         <v>0.19807549962990378</v>
       </c>
@@ -5093,7 +5098,7 @@
       <c r="D89" t="s">
         <v>4</v>
       </c>
-      <c r="E89" s="72">
+      <c r="E89" s="56">
         <f>'ShareOfInflow-SEIS'!K18</f>
         <v>0.19700563296768453</v>
       </c>
@@ -5114,7 +5119,7 @@
       <c r="D90" t="s">
         <v>4</v>
       </c>
-      <c r="E90" s="72">
+      <c r="E90" s="56">
         <f>'ShareOfInflow-SEIS'!K19</f>
         <v>0.18443239987955437</v>
       </c>
@@ -5135,7 +5140,7 @@
       <c r="D91" t="s">
         <v>4</v>
       </c>
-      <c r="E91" s="72">
+      <c r="E91" s="56">
         <f>'ShareOfInflow-SEIS'!P12</f>
         <v>0.17046383923355535</v>
       </c>
@@ -5156,7 +5161,7 @@
       <c r="D92" t="s">
         <v>4</v>
       </c>
-      <c r="E92" s="72">
+      <c r="E92" s="56">
         <f>'ShareOfInflow-SEIS'!P13</f>
         <v>0.18079959256429842</v>
       </c>
@@ -5177,7 +5182,7 @@
       <c r="D93" t="s">
         <v>4</v>
       </c>
-      <c r="E93" s="72">
+      <c r="E93" s="56">
         <f>'ShareOfInflow-SEIS'!P14</f>
         <v>0.18219785956669277</v>
       </c>
@@ -5198,7 +5203,7 @@
       <c r="D94" t="s">
         <v>4</v>
       </c>
-      <c r="E94" s="72">
+      <c r="E94" s="56">
         <f>'ShareOfInflow-SEIS'!P15</f>
         <v>0.19016853932584271</v>
       </c>
@@ -5219,7 +5224,7 @@
       <c r="D95" t="s">
         <v>4</v>
       </c>
-      <c r="E95" s="72">
+      <c r="E95" s="56">
         <f>'ShareOfInflow-SEIS'!P16</f>
         <v>0.19195664575014262</v>
       </c>
@@ -5240,7 +5245,7 @@
       <c r="D96" t="s">
         <v>4</v>
       </c>
-      <c r="E96" s="72">
+      <c r="E96" s="56">
         <f>'ShareOfInflow-SEIS'!P17</f>
         <v>0.19380069524913096</v>
       </c>
@@ -5261,7 +5266,7 @@
       <c r="D97" t="s">
         <v>4</v>
       </c>
-      <c r="E97" s="72">
+      <c r="E97" s="56">
         <f>'ShareOfInflow-SEIS'!P18</f>
         <v>0.19558498896247239</v>
       </c>
@@ -5282,7 +5287,7 @@
       <c r="D98" t="s">
         <v>4</v>
       </c>
-      <c r="E98" s="72">
+      <c r="E98" s="56">
         <f>'ShareOfInflow-SEIS'!P19</f>
         <v>0.18773946360153257</v>
       </c>
@@ -5351,134 +5356,134 @@
       <c r="B10" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="64" t="str">
+      <c r="C10" s="59" t="str">
         <f>'SEIS-Cuts'!I7</f>
         <v>Alternative 1 - Priority</v>
       </c>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="68" t="s">
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="I10" s="68"/>
-      <c r="J10" s="68"/>
-      <c r="K10" s="68"/>
-      <c r="L10" s="68"/>
-      <c r="M10" s="55" t="s">
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="55"/>
-      <c r="Q10" s="55"/>
+      <c r="N10" s="61"/>
+      <c r="O10" s="61"/>
+      <c r="P10" s="61"/>
+      <c r="Q10" s="61"/>
     </row>
     <row r="11" spans="1:17" s="21" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="62"/>
       <c r="B11" s="63"/>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="65" t="s">
+      <c r="D11" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="65" t="s">
+      <c r="E11" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="65" t="s">
+      <c r="F11" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="65" t="s">
+      <c r="G11" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="69" t="str">
+      <c r="H11" s="53" t="str">
         <f>C11</f>
         <v>Arizona</v>
       </c>
-      <c r="I11" s="69" t="str">
+      <c r="I11" s="53" t="str">
         <f t="shared" ref="I11:L11" si="0">D11</f>
         <v>Nevada</v>
       </c>
-      <c r="J11" s="69" t="str">
+      <c r="J11" s="53" t="str">
         <f t="shared" si="0"/>
         <v>California</v>
       </c>
-      <c r="K11" s="69" t="str">
+      <c r="K11" s="53" t="str">
         <f t="shared" si="0"/>
         <v>Mexico</v>
       </c>
-      <c r="L11" s="69" t="str">
+      <c r="L11" s="53" t="str">
         <f t="shared" si="0"/>
         <v>Total</v>
       </c>
-      <c r="M11" s="54" t="str">
+      <c r="M11" s="45" t="str">
         <f>H11</f>
         <v>Arizona</v>
       </c>
-      <c r="N11" s="54" t="str">
+      <c r="N11" s="45" t="str">
         <f t="shared" ref="N11" si="1">I11</f>
         <v>Nevada</v>
       </c>
-      <c r="O11" s="54" t="str">
+      <c r="O11" s="45" t="str">
         <f t="shared" ref="O11" si="2">J11</f>
         <v>California</v>
       </c>
-      <c r="P11" s="54" t="str">
+      <c r="P11" s="45" t="str">
         <f t="shared" ref="P11" si="3">K11</f>
         <v>Mexico</v>
       </c>
-      <c r="Q11" s="54" t="str">
+      <c r="Q11" s="45" t="str">
         <f t="shared" ref="Q11" si="4">L11</f>
         <v>Total</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" s="60" t="str">
+      <c r="A12" s="49" t="str">
         <f>'SEIS-Cuts'!A10</f>
         <v>1,090–&gt;1,075</v>
       </c>
-      <c r="B12" s="61">
+      <c r="B12" s="50">
         <f>'SEIS-Cuts'!B10</f>
         <v>10.857008</v>
       </c>
-      <c r="C12" s="66">
+      <c r="C12" s="52">
         <f>(C$9-'SEIS-Cuts'!O10/1000)/($G$9-'SEIS-Cuts'!$T10/1000)</f>
         <v>0.2822759668185536</v>
       </c>
-      <c r="D12" s="66">
+      <c r="D12" s="52">
         <f>(D$9-'SEIS-Cuts'!P10/1000)/($G$9-'SEIS-Cuts'!$T10/1000)</f>
         <v>3.3181446430657784E-2</v>
       </c>
-      <c r="E12" s="66">
+      <c r="E12" s="52">
         <f>(E$9-'SEIS-Cuts'!Q10/1000)/($G$9-'SEIS-Cuts'!$T10/1000)</f>
         <v>0.51407874751723337</v>
       </c>
-      <c r="F12" s="66">
+      <c r="F12" s="52">
         <f>(F$9-'SEIS-Cuts'!S10/1000)/($G$9-'SEIS-Cuts'!$T10/1000)</f>
         <v>0.17046383923355535</v>
       </c>
-      <c r="G12" s="67">
+      <c r="G12" s="52">
         <f>(G$9-'SEIS-Cuts'!T10)/($G$9-SUM('SEIS-Cuts'!O10:Q10,'SEIS-Cuts'!S10))</f>
         <v>1</v>
       </c>
-      <c r="H12" s="70">
+      <c r="H12" s="54">
         <f>(C$9-'SEIS-Cuts'!Z10/1000)/($G$9-'SEIS-Cuts'!$AE10/1000)</f>
         <v>0.29594578805935273</v>
       </c>
-      <c r="I12" s="70">
+      <c r="I12" s="54">
         <f>(D$9-'SEIS-Cuts'!AA10/1000)/($G$9-'SEIS-Cuts'!$AE10/1000)</f>
         <v>3.3181446430657784E-2</v>
       </c>
-      <c r="J12" s="70">
+      <c r="J12" s="54">
         <f>(E$9-'SEIS-Cuts'!AB10/1000)/($G$9-'SEIS-Cuts'!$AE10/1000)</f>
         <v>0.5004089262764343</v>
       </c>
-      <c r="K12" s="70">
+      <c r="K12" s="54">
         <f>(F$9-'SEIS-Cuts'!AD10/1000)/($G$9-'SEIS-Cuts'!$AE10/1000)</f>
         <v>0.17046383923355535</v>
       </c>
-      <c r="L12" s="70">
+      <c r="L12" s="54">
         <f>(G$9-'SEIS-Cuts'!AE10/1000)/($G$9-'SEIS-Cuts'!$AE10/1000)</f>
         <v>1</v>
       </c>
@@ -5504,51 +5509,51 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="60" t="str">
+      <c r="A13" s="49" t="str">
         <f>'SEIS-Cuts'!A11</f>
         <v>1,075–1,050</v>
       </c>
-      <c r="B13" s="61">
+      <c r="B13" s="50">
         <f>'SEIS-Cuts'!B11</f>
         <v>9.6009879999900001</v>
       </c>
-      <c r="C13" s="66">
+      <c r="C13" s="52">
         <f>(C$9-'SEIS-Cuts'!O11/1000)/($G$9-'SEIS-Cuts'!$T11/1000)</f>
         <v>0.22625413801884389</v>
       </c>
-      <c r="D13" s="66">
+      <c r="D13" s="52">
         <f>(D$9-'SEIS-Cuts'!P11/1000)/($G$9-'SEIS-Cuts'!$T11/1000)</f>
         <v>3.2722179781003308E-2</v>
       </c>
-      <c r="E13" s="66">
+      <c r="E13" s="52">
         <f>(E$9-'SEIS-Cuts'!Q11/1000)/($G$9-'SEIS-Cuts'!$T11/1000)</f>
         <v>0.56022408963585435</v>
       </c>
-      <c r="F13" s="66">
+      <c r="F13" s="52">
         <f>(F$9-'SEIS-Cuts'!S11/1000)/($G$9-'SEIS-Cuts'!$T11/1000)</f>
         <v>0.18079959256429842</v>
       </c>
-      <c r="G13" s="67">
+      <c r="G13" s="52">
         <f>(G$9-'SEIS-Cuts'!T11)/($G$9-SUM('SEIS-Cuts'!O11:Q11,'SEIS-Cuts'!S11))</f>
         <v>1</v>
       </c>
-      <c r="H13" s="70">
+      <c r="H13" s="54">
         <f>(C$9-'SEIS-Cuts'!Z11/1000)/($G$9-'SEIS-Cuts'!$AE11/1000)</f>
         <v>0.26597911892029541</v>
       </c>
-      <c r="I13" s="70">
+      <c r="I13" s="54">
         <f>(D$9-'SEIS-Cuts'!AA11/1000)/($G$9-'SEIS-Cuts'!$AE11/1000)</f>
         <v>3.2849503437738729E-2</v>
       </c>
-      <c r="J13" s="70">
+      <c r="J13" s="54">
         <f>(E$9-'SEIS-Cuts'!AB11/1000)/($G$9-'SEIS-Cuts'!$AE11/1000)</f>
         <v>0.52037178507766746</v>
       </c>
-      <c r="K13" s="70">
+      <c r="K13" s="54">
         <f>(F$9-'SEIS-Cuts'!AD11/1000)/($G$9-'SEIS-Cuts'!$AE11/1000)</f>
         <v>0.18079959256429842</v>
       </c>
-      <c r="L13" s="70">
+      <c r="L13" s="54">
         <f>(G$9-'SEIS-Cuts'!AE11/1000)/($G$9-'SEIS-Cuts'!$AE11/1000)</f>
         <v>1</v>
       </c>
@@ -5574,51 +5579,51 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A14" s="60" t="str">
+      <c r="A14" s="49" t="str">
         <f>'SEIS-Cuts'!A12</f>
         <v>&lt;1,050–&gt;1,045</v>
       </c>
-      <c r="B14" s="61">
+      <c r="B14" s="50">
         <f>'SEIS-Cuts'!B12</f>
         <v>7.6828779999999997</v>
       </c>
-      <c r="C14" s="66">
+      <c r="C14" s="52">
         <f>(C$9-'SEIS-Cuts'!O12/1000)/($G$9-'SEIS-Cuts'!$T12/1000)</f>
         <v>0.2107804750717828</v>
       </c>
-      <c r="D14" s="66">
+      <c r="D14" s="52">
         <f>(D$9-'SEIS-Cuts'!P12/1000)/($G$9-'SEIS-Cuts'!$T12/1000)</f>
         <v>3.2759070738710518E-2</v>
       </c>
-      <c r="E14" s="66">
+      <c r="E14" s="52">
         <f>(E$9-'SEIS-Cuts'!Q12/1000)/($G$9-'SEIS-Cuts'!$T12/1000)</f>
         <v>0.57426259462281393</v>
       </c>
-      <c r="F14" s="66">
+      <c r="F14" s="52">
         <f>(F$9-'SEIS-Cuts'!S12/1000)/($G$9-'SEIS-Cuts'!$T12/1000)</f>
         <v>0.18219785956669277</v>
       </c>
-      <c r="G14" s="67">
+      <c r="G14" s="52">
         <f>(G$9-'SEIS-Cuts'!T12)/($G$9-SUM('SEIS-Cuts'!O12:Q12,'SEIS-Cuts'!S12))</f>
         <v>1</v>
       </c>
-      <c r="H14" s="70">
+      <c r="H14" s="54">
         <f>(C$9-'SEIS-Cuts'!Z12/1000)/($G$9-'SEIS-Cuts'!$AE12/1000)</f>
         <v>0.25815713912816496</v>
       </c>
-      <c r="I14" s="70">
+      <c r="I14" s="54">
         <f>(D$9-'SEIS-Cuts'!AA12/1000)/($G$9-'SEIS-Cuts'!$AE12/1000)</f>
         <v>3.2628556512659883E-2</v>
       </c>
-      <c r="J14" s="70">
+      <c r="J14" s="54">
         <f>(E$9-'SEIS-Cuts'!AB12/1000)/($G$9-'SEIS-Cuts'!$AE12/1000)</f>
         <v>0.52701644479248244</v>
       </c>
-      <c r="K14" s="70">
+      <c r="K14" s="54">
         <f>(F$9-'SEIS-Cuts'!AD12/1000)/($G$9-'SEIS-Cuts'!$AE12/1000)</f>
         <v>0.18219785956669277</v>
       </c>
-      <c r="L14" s="70">
+      <c r="L14" s="54">
         <f>(G$9-'SEIS-Cuts'!AE12/1000)/($G$9-'SEIS-Cuts'!$AE12/1000)</f>
         <v>1</v>
       </c>
@@ -5644,51 +5649,51 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="60" t="str">
+      <c r="A15" s="49" t="str">
         <f>'SEIS-Cuts'!A13</f>
         <v>1,045–&gt;1,040</v>
       </c>
-      <c r="B15" s="61">
+      <c r="B15" s="50">
         <f>'SEIS-Cuts'!B13</f>
         <v>7.3260519999999998</v>
       </c>
-      <c r="C15" s="66">
+      <c r="C15" s="52">
         <f>(C$9-'SEIS-Cuts'!O13/1000)/($G$9-'SEIS-Cuts'!$T13/1000)</f>
         <v>0.16401734104046239</v>
       </c>
-      <c r="D15" s="66">
+      <c r="D15" s="52">
         <f>(D$9-'SEIS-Cuts'!P13/1000)/($G$9-'SEIS-Cuts'!$T13/1000)</f>
         <v>3.3381502890173408E-2</v>
       </c>
-      <c r="E15" s="66">
+      <c r="E15" s="52">
         <f>(E$9-'SEIS-Cuts'!Q13/1000)/($G$9-'SEIS-Cuts'!$T13/1000)</f>
         <v>0.60693641618497118</v>
       </c>
-      <c r="F15" s="66">
+      <c r="F15" s="52">
         <f>(F$9-'SEIS-Cuts'!S13/1000)/($G$9-'SEIS-Cuts'!$T13/1000)</f>
         <v>0.19566473988439309</v>
       </c>
-      <c r="G15" s="67">
+      <c r="G15" s="52">
         <f>(G$9-'SEIS-Cuts'!T13)/($G$9-SUM('SEIS-Cuts'!O13:Q13,'SEIS-Cuts'!S13))</f>
         <v>1</v>
       </c>
-      <c r="H15" s="70">
+      <c r="H15" s="54">
         <f>(C$9-'SEIS-Cuts'!Z13/1000)/($G$9-'SEIS-Cuts'!$AE13/1000)</f>
         <v>0.25786516853932584</v>
       </c>
-      <c r="I15" s="70">
+      <c r="I15" s="54">
         <f>(D$9-'SEIS-Cuts'!AA13/1000)/($G$9-'SEIS-Cuts'!$AE13/1000)</f>
         <v>3.3426966292134833E-2</v>
       </c>
-      <c r="J15" s="70">
+      <c r="J15" s="54">
         <f>(E$9-'SEIS-Cuts'!AB13/1000)/($G$9-'SEIS-Cuts'!$AE13/1000)</f>
         <v>0.51839887640449445</v>
       </c>
-      <c r="K15" s="70">
+      <c r="K15" s="54">
         <f>(F$9-'SEIS-Cuts'!AD13/1000)/($G$9-'SEIS-Cuts'!$AE13/1000)</f>
         <v>0.19016853932584271</v>
       </c>
-      <c r="L15" s="70">
+      <c r="L15" s="54">
         <f>(G$9-'SEIS-Cuts'!AE13/1000)/($G$9-'SEIS-Cuts'!$AE13/1000)</f>
         <v>1</v>
       </c>
@@ -5714,51 +5719,51 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A16" s="60" t="str">
+      <c r="A16" s="49" t="str">
         <f>'SEIS-Cuts'!A14</f>
         <v>1,040–&gt;1,035</v>
       </c>
-      <c r="B16" s="61">
+      <c r="B16" s="50">
         <f>'SEIS-Cuts'!B14</f>
         <v>6.977665</v>
       </c>
-      <c r="C16" s="66">
+      <c r="C16" s="52">
         <f>(C$9-'SEIS-Cuts'!O14/1000)/($G$9-'SEIS-Cuts'!$T14/1000)</f>
         <v>0.15703090344521659</v>
       </c>
-      <c r="D16" s="66">
+      <c r="D16" s="52">
         <f>(D$9-'SEIS-Cuts'!P14/1000)/($G$9-'SEIS-Cuts'!$T14/1000)</f>
         <v>3.2086352210557438E-2</v>
       </c>
-      <c r="E16" s="66">
+      <c r="E16" s="52">
         <f>(E$9-'SEIS-Cuts'!Q14/1000)/($G$9-'SEIS-Cuts'!$T14/1000)</f>
         <v>0.6118586426142244</v>
       </c>
-      <c r="F16" s="66">
+      <c r="F16" s="52">
         <f>(F$9-'SEIS-Cuts'!S14/1000)/($G$9-'SEIS-Cuts'!$T14/1000)</f>
         <v>0.19902410173000148</v>
       </c>
-      <c r="G16" s="67">
+      <c r="G16" s="52">
         <f>(G$9-'SEIS-Cuts'!T14)/($G$9-SUM('SEIS-Cuts'!O14:Q14,'SEIS-Cuts'!S14))</f>
         <v>1</v>
       </c>
-      <c r="H16" s="70">
+      <c r="H16" s="54">
         <f>(C$9-'SEIS-Cuts'!Z14/1000)/($G$9-'SEIS-Cuts'!$AE14/1000)</f>
         <v>0.25506432056779532</v>
       </c>
-      <c r="I16" s="70">
+      <c r="I16" s="54">
         <f>(D$9-'SEIS-Cuts'!AA14/1000)/($G$9-'SEIS-Cuts'!$AE14/1000)</f>
         <v>3.3417122578737246E-2</v>
       </c>
-      <c r="J16" s="70">
+      <c r="J16" s="54">
         <f>(E$9-'SEIS-Cuts'!AB14/1000)/($G$9-'SEIS-Cuts'!$AE14/1000)</f>
         <v>0.51249445512346592</v>
       </c>
-      <c r="K16" s="70">
+      <c r="K16" s="54">
         <f>(F$9-'SEIS-Cuts'!AD14/1000)/($G$9-'SEIS-Cuts'!$AE14/1000)</f>
         <v>0.19902410173000148</v>
       </c>
-      <c r="L16" s="70">
+      <c r="L16" s="54">
         <f>(G$9-'SEIS-Cuts'!AE14/1000)/($G$9-'SEIS-Cuts'!$AE14/1000)</f>
         <v>1</v>
       </c>
@@ -5784,51 +5789,51 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A17" s="60" t="str">
+      <c r="A17" s="49" t="str">
         <f>'SEIS-Cuts'!A15</f>
         <v>1,035–&gt;1,030</v>
       </c>
-      <c r="B17" s="61">
+      <c r="B17" s="50">
         <f>'SEIS-Cuts'!B15</f>
         <v>6.6375080000000004</v>
       </c>
-      <c r="C17" s="66">
+      <c r="C17" s="52">
         <f>(C$9-'SEIS-Cuts'!O15/1000)/($G$9-'SEIS-Cuts'!$T15/1000)</f>
         <v>0.15810629745422058</v>
       </c>
-      <c r="D17" s="66">
+      <c r="D17" s="52">
         <f>(D$9-'SEIS-Cuts'!P15/1000)/($G$9-'SEIS-Cuts'!$T15/1000)</f>
         <v>3.2306089027839803E-2</v>
       </c>
-      <c r="E17" s="66">
+      <c r="E17" s="52">
         <f>(E$9-'SEIS-Cuts'!Q15/1000)/($G$9-'SEIS-Cuts'!$T15/1000)</f>
         <v>0.61039154384397798</v>
       </c>
-      <c r="F17" s="66">
+      <c r="F17" s="52">
         <f>(F$9-'SEIS-Cuts'!S15/1000)/($G$9-'SEIS-Cuts'!$T15/1000)</f>
         <v>0.19919606967396158</v>
       </c>
-      <c r="G17" s="67">
+      <c r="G17" s="52">
         <f>(G$9-'SEIS-Cuts'!T15)/($G$9-SUM('SEIS-Cuts'!O15:Q15,'SEIS-Cuts'!S15))</f>
         <v>1</v>
       </c>
-      <c r="H17" s="70">
+      <c r="H17" s="54">
         <f>(C$9-'SEIS-Cuts'!Z15/1000)/($G$9-'SEIS-Cuts'!$AE15/1000)</f>
         <v>0.25803108808290154</v>
       </c>
-      <c r="I17" s="70">
+      <c r="I17" s="54">
         <f>(D$9-'SEIS-Cuts'!AA15/1000)/($G$9-'SEIS-Cuts'!$AE15/1000)</f>
         <v>3.3752775721687639E-2</v>
       </c>
-      <c r="J17" s="70">
+      <c r="J17" s="54">
         <f>(E$9-'SEIS-Cuts'!AB15/1000)/($G$9-'SEIS-Cuts'!$AE15/1000)</f>
         <v>0.50999259807549968</v>
       </c>
-      <c r="K17" s="70">
+      <c r="K17" s="54">
         <f>(F$9-'SEIS-Cuts'!AD15/1000)/($G$9-'SEIS-Cuts'!$AE15/1000)</f>
         <v>0.19807549962990378</v>
       </c>
-      <c r="L17" s="70">
+      <c r="L17" s="54">
         <f>(G$9-'SEIS-Cuts'!AE15/1000)/($G$9-'SEIS-Cuts'!$AE15/1000)</f>
         <v>1</v>
       </c>
@@ -5854,51 +5859,51 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A18" s="60" t="str">
+      <c r="A18" s="49" t="str">
         <f>'SEIS-Cuts'!A16</f>
         <v>1,030–1,025</v>
       </c>
-      <c r="B18" s="61">
+      <c r="B18" s="50">
         <f>'SEIS-Cuts'!B16</f>
         <v>6.305377</v>
       </c>
-      <c r="C18" s="66">
+      <c r="C18" s="52">
         <f>(C$9-'SEIS-Cuts'!O16/1000)/($G$9-'SEIS-Cuts'!$T16/1000)</f>
         <v>0.15950735956743767</v>
       </c>
-      <c r="D18" s="66">
+      <c r="D18" s="52">
         <f>(D$9-'SEIS-Cuts'!P16/1000)/($G$9-'SEIS-Cuts'!$T16/1000)</f>
         <v>3.2592370081105437E-2</v>
       </c>
-      <c r="E18" s="66">
+      <c r="E18" s="52">
         <f>(E$9-'SEIS-Cuts'!Q16/1000)/($G$9-'SEIS-Cuts'!$T16/1000)</f>
         <v>0.60829077801141496</v>
       </c>
-      <c r="F18" s="66">
+      <c r="F18" s="52">
         <f>(F$9-'SEIS-Cuts'!S16/1000)/($G$9-'SEIS-Cuts'!$T16/1000)</f>
         <v>0.19960949234004208</v>
       </c>
-      <c r="G18" s="67">
+      <c r="G18" s="52">
         <f>(G$9-'SEIS-Cuts'!T16)/($G$9-SUM('SEIS-Cuts'!O16:Q16,'SEIS-Cuts'!S16))</f>
         <v>1</v>
       </c>
-      <c r="H18" s="70">
+      <c r="H18" s="54">
         <f>(C$9-'SEIS-Cuts'!Z16/1000)/($G$9-'SEIS-Cuts'!$AE16/1000)</f>
         <v>0.26119181737325819</v>
       </c>
-      <c r="I18" s="70">
+      <c r="I18" s="54">
         <f>(D$9-'SEIS-Cuts'!AA16/1000)/($G$9-'SEIS-Cuts'!$AE16/1000)</f>
         <v>3.4094278090720423E-2</v>
       </c>
-      <c r="J18" s="70">
+      <c r="J18" s="54">
         <f>(E$9-'SEIS-Cuts'!AB16/1000)/($G$9-'SEIS-Cuts'!$AE16/1000)</f>
         <v>0.50770827156833676</v>
       </c>
-      <c r="K18" s="70">
+      <c r="K18" s="54">
         <f>(F$9-'SEIS-Cuts'!AD16/1000)/($G$9-'SEIS-Cuts'!$AE16/1000)</f>
         <v>0.19700563296768453</v>
       </c>
-      <c r="L18" s="70">
+      <c r="L18" s="54">
         <f>(G$9-'SEIS-Cuts'!AE16/1000)/($G$9-'SEIS-Cuts'!$AE16/1000)</f>
         <v>1</v>
       </c>
@@ -5924,51 +5929,51 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A19" s="60" t="str">
+      <c r="A19" s="49" t="str">
         <f>'SEIS-Cuts'!A17</f>
         <v>&lt;1,025–1,000</v>
       </c>
-      <c r="B19" s="61">
+      <c r="B19" s="50">
         <f>'SEIS-Cuts'!B17</f>
         <v>5.981122</v>
       </c>
-      <c r="C19" s="66">
+      <c r="C19" s="52">
         <f>(C$9-'SEIS-Cuts'!O17/1000)/($G$9-'SEIS-Cuts'!$T17/1000)</f>
         <v>0.1620384498016478</v>
       </c>
-      <c r="D19" s="66">
+      <c r="D19" s="52">
         <f>(D$9-'SEIS-Cuts'!P17/1000)/($G$9-'SEIS-Cuts'!$T17/1000)</f>
         <v>3.3109551418980768E-2</v>
       </c>
-      <c r="E19" s="66">
+      <c r="E19" s="52">
         <f>(E$9-'SEIS-Cuts'!Q17/1000)/($G$9-'SEIS-Cuts'!$T17/1000)</f>
         <v>0.61794324076899609</v>
       </c>
-      <c r="F19" s="66">
+      <c r="F19" s="52">
         <f>(F$9-'SEIS-Cuts'!S17/1000)/($G$9-'SEIS-Cuts'!$T17/1000)</f>
         <v>0.18690875801037535</v>
       </c>
-      <c r="G19" s="67">
+      <c r="G19" s="52">
         <f>(G$9-'SEIS-Cuts'!T17)/($G$9-SUM('SEIS-Cuts'!O17:Q17,'SEIS-Cuts'!S17))</f>
         <v>1</v>
       </c>
-      <c r="H19" s="70">
+      <c r="H19" s="54">
         <f>(C$9-'SEIS-Cuts'!Z17/1000)/($G$9-'SEIS-Cuts'!$AE17/1000)</f>
         <v>0.25790424570912374</v>
       </c>
-      <c r="I19" s="70">
+      <c r="I19" s="54">
         <f>(D$9-'SEIS-Cuts'!AA17/1000)/($G$9-'SEIS-Cuts'!$AE17/1000)</f>
         <v>3.4778681120144532E-2</v>
       </c>
-      <c r="J19" s="70">
+      <c r="J19" s="54">
         <f>(E$9-'SEIS-Cuts'!AB17/1000)/($G$9-'SEIS-Cuts'!$AE17/1000)</f>
         <v>0.52288467329117749</v>
       </c>
-      <c r="K19" s="70">
+      <c r="K19" s="54">
         <f>(F$9-'SEIS-Cuts'!AD17/1000)/($G$9-'SEIS-Cuts'!$AE17/1000)</f>
         <v>0.18443239987955437</v>
       </c>
-      <c r="L19" s="70">
+      <c r="L19" s="54">
         <f>(G$9-'SEIS-Cuts'!AE17/1000)/($G$9-'SEIS-Cuts'!$AE17/1000)</f>
         <v>1</v>
       </c>
@@ -6012,8 +6017,8 @@
         <f>'SEIS-Cuts'!B19</f>
         <v>0</v>
       </c>
-      <c r="G21" s="56"/>
-      <c r="L21" s="56"/>
+      <c r="G21" s="46"/>
+      <c r="L21" s="46"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="22" t="str">
@@ -6024,43 +6029,43 @@
         <f>'SEIS-Cuts'!B20</f>
         <v>0</v>
       </c>
-      <c r="G22" s="56"/>
-      <c r="L22" s="56"/>
+      <c r="G22" s="46"/>
+      <c r="L22" s="46"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="G23" s="56"/>
-      <c r="L23" s="56"/>
+      <c r="G23" s="46"/>
+      <c r="L23" s="46"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="G24" s="56"/>
-      <c r="L24" s="56"/>
+      <c r="G24" s="46"/>
+      <c r="L24" s="46"/>
     </row>
     <row r="25" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="58"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="59"/>
-      <c r="L25" s="56"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="48"/>
+      <c r="L25" s="46"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="G26" s="56"/>
-      <c r="L26" s="56"/>
+      <c r="G26" s="46"/>
+      <c r="L26" s="46"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="G27" s="56"/>
-      <c r="L27" s="56"/>
+      <c r="G27" s="46"/>
+      <c r="L27" s="46"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="G28" s="56"/>
-      <c r="L28" s="56"/>
+      <c r="G28" s="46"/>
+      <c r="L28" s="46"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="G29" s="56"/>
+      <c r="G29" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6140,96 +6145,96 @@
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="52" t="s">
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="52"/>
-      <c r="S7" s="52"/>
-      <c r="T7" s="52"/>
-      <c r="U7" s="52" t="s">
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="66"/>
+      <c r="N7" s="66"/>
+      <c r="O7" s="66"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="66"/>
+      <c r="R7" s="66"/>
+      <c r="S7" s="66"/>
+      <c r="T7" s="66"/>
+      <c r="U7" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="V7" s="52"/>
-      <c r="W7" s="52"/>
-      <c r="X7" s="52"/>
-      <c r="Y7" s="52"/>
-      <c r="Z7" s="52"/>
-      <c r="AA7" s="52"/>
-      <c r="AB7" s="52"/>
-      <c r="AC7" s="52"/>
+      <c r="V7" s="66"/>
+      <c r="W7" s="66"/>
+      <c r="X7" s="66"/>
+      <c r="Y7" s="66"/>
+      <c r="Z7" s="66"/>
+      <c r="AA7" s="66"/>
+      <c r="AB7" s="66"/>
+      <c r="AC7" s="66"/>
       <c r="AD7" s="42"/>
       <c r="AE7" s="42"/>
-      <c r="AF7" s="52" t="s">
+      <c r="AF7" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="AG7" s="52"/>
+      <c r="AG7" s="66"/>
     </row>
     <row r="8" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="45"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="46" t="s">
+      <c r="A8" s="67"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="46" t="s">
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="69"/>
+      <c r="N8" s="69"/>
+      <c r="O8" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="46"/>
-      <c r="S8" s="46"/>
-      <c r="T8" s="46"/>
-      <c r="U8" s="47" t="s">
+      <c r="P8" s="69"/>
+      <c r="Q8" s="69"/>
+      <c r="R8" s="69"/>
+      <c r="S8" s="69"/>
+      <c r="T8" s="69"/>
+      <c r="U8" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="V8" s="47"/>
-      <c r="W8" s="47"/>
-      <c r="X8" s="47"/>
-      <c r="Y8" s="47"/>
-      <c r="Z8" s="50" t="s">
+      <c r="V8" s="70"/>
+      <c r="W8" s="70"/>
+      <c r="X8" s="70"/>
+      <c r="Y8" s="70"/>
+      <c r="Z8" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="AA8" s="57"/>
-      <c r="AB8" s="57"/>
-      <c r="AC8" s="57"/>
-      <c r="AD8" s="57"/>
-      <c r="AE8" s="51"/>
-      <c r="AF8" s="50" t="s">
+      <c r="AA8" s="68"/>
+      <c r="AB8" s="68"/>
+      <c r="AC8" s="68"/>
+      <c r="AD8" s="68"/>
+      <c r="AE8" s="65"/>
+      <c r="AF8" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="AG8" s="51"/>
+      <c r="AG8" s="65"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" s="41"/>
@@ -6495,7 +6500,7 @@
         <v>0</v>
       </c>
       <c r="R11" s="12">
-        <f t="shared" ref="R11:R20" si="4">F11+L11</f>
+        <f t="shared" ref="R11:R19" si="4">F11+L11</f>
         <v>1066</v>
       </c>
       <c r="S11" s="12">
@@ -6534,11 +6539,11 @@
         <v>1066</v>
       </c>
       <c r="AD11" s="12">
-        <f t="shared" ref="AD11:AD33" si="7">G11</f>
+        <f t="shared" ref="AD11:AD20" si="7">G11</f>
         <v>80</v>
       </c>
       <c r="AE11" s="12">
-        <f t="shared" ref="AE11:AE33" si="8">AC11+AD11</f>
+        <f t="shared" ref="AE11:AE20" si="8">AC11+AD11</f>
         <v>1146</v>
       </c>
       <c r="AF11" s="12">
@@ -7773,17 +7778,17 @@
     <sortCondition descending="1" ref="B10:B17"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="O8:T8"/>
+    <mergeCell ref="U8:Y8"/>
+    <mergeCell ref="B7:B8"/>
     <mergeCell ref="AF8:AG8"/>
     <mergeCell ref="AF7:AG7"/>
     <mergeCell ref="I7:T7"/>
     <mergeCell ref="U7:AC7"/>
     <mergeCell ref="C7:H8"/>
     <mergeCell ref="Z8:AE8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="I8:N8"/>
-    <mergeCell ref="O8:T8"/>
-    <mergeCell ref="U8:Y8"/>
-    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{37A0A559-A066-48B0-9816-F9F7E3B09C10}"/>
@@ -7827,25 +7832,25 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53" t="s">
+      <c r="E3" s="73"/>
+      <c r="F3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53" t="s">
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="M3" s="53" t="s">
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="M3" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
     </row>
     <row r="4" spans="1:16" s="4" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
@@ -9531,7 +9536,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="O21" s="56"/>
+      <c r="O21" s="46"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">

</xml_diff>

<commit_message>
Add percent allocation at full allocations
</commit_message>
<xml_diff>
--- a/MeadInflowSplit/ShareOfInflow-LB-MX-SEIS.xlsx
+++ b/MeadInflowSplit/ShareOfInflow-LB-MX-SEIS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\MeadInflowSplit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9590CB-2F5F-474A-B63D-8BFDD641AEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E61B7A-6ECE-4C99-BE35-1D52FB7D3A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{B7E24150-B936-4491-85FE-E2B15A6311EA}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{B7E24150-B936-4491-85FE-E2B15A6311EA}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="7" r:id="rId1"/>
@@ -759,7 +759,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -901,6 +901,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -916,19 +925,7 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -943,17 +940,23 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -962,115 +965,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <alignment horizontal="center"/>
     </dxf>
@@ -1100,18 +995,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
@@ -2218,7 +2101,7 @@
     <dataField name="Sum of Percent of Total" fld="4" baseField="0" baseItem="0" numFmtId="9"/>
   </dataFields>
   <formats count="12">
-    <format dxfId="51">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1">
@@ -2230,14 +2113,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="10">
       <pivotArea dataOnly="0" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="9">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -2246,26 +2129,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="8">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="7">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="6">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="5">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="0"/>
@@ -2275,7 +2158,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="0"/>
@@ -2285,7 +2168,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="0"/>
@@ -2295,7 +2178,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="0"/>
@@ -2783,7 +2666,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -2874,11 +2757,11 @@
   <sheetData>
     <row r="2" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="55" t="str">
-        <f>'ShareOfInflow-SEIS'!A10</f>
+        <f>'ShareOfInflow-SEIS'!A11</f>
         <v>Mead Elevation (feet)</v>
       </c>
       <c r="B2" s="55" t="str">
-        <f>'ShareOfInflow-SEIS'!B10</f>
+        <f>'ShareOfInflow-SEIS'!B11</f>
         <v>Mead Volume (maf)</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2893,28 +2776,28 @@
       <c r="H2" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="74" t="s">
+      <c r="I2" s="59" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
-        <f>'ShareOfInflow-SEIS'!A12</f>
+        <f>'ShareOfInflow-SEIS'!A13</f>
         <v>1,090–&gt;1,075</v>
       </c>
       <c r="B3" s="7">
-        <f>'ShareOfInflow-SEIS'!B12</f>
+        <f>'ShareOfInflow-SEIS'!B13</f>
         <v>10.857008</v>
       </c>
       <c r="C3" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="56">
-        <f>'ShareOfInflow-SEIS'!C12</f>
+        <f>'ShareOfInflow-SEIS'!C13</f>
         <v>0.2822759668185536</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -2932,421 +2815,421 @@
     </row>
     <row r="4" spans="1:20" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
-        <f>'ShareOfInflow-SEIS'!A13</f>
+        <f>'ShareOfInflow-SEIS'!A14</f>
         <v>1,075–1,050</v>
       </c>
       <c r="B4" s="7">
-        <f>'ShareOfInflow-SEIS'!B13</f>
+        <f>'ShareOfInflow-SEIS'!B14</f>
         <v>9.6009879999900001</v>
       </c>
       <c r="C4" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="56">
-        <f>'ShareOfInflow-SEIS'!C13</f>
+        <f>'ShareOfInflow-SEIS'!C14</f>
         <v>0.22625413801884389</v>
       </c>
       <c r="H4" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="I4" s="75" t="s">
+      <c r="I4" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="75" t="s">
+      <c r="J4" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="75" t="s">
+      <c r="K4" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="L4" s="75" t="s">
+      <c r="L4" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="M4" s="75" t="s">
+      <c r="M4" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="N4" s="75" t="s">
+      <c r="N4" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="O4" s="75" t="s">
+      <c r="O4" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="P4" s="75" t="s">
+      <c r="P4" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="Q4" s="75" t="s">
+      <c r="Q4" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="R4" s="75" t="s">
+      <c r="R4" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="S4" s="75" t="s">
+      <c r="S4" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="T4" s="75" t="s">
+      <c r="T4" s="60" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
-        <f>'ShareOfInflow-SEIS'!A14</f>
+        <f>'ShareOfInflow-SEIS'!A15</f>
         <v>&lt;1,050–&gt;1,045</v>
       </c>
       <c r="B5" s="7">
-        <f>'ShareOfInflow-SEIS'!B14</f>
+        <f>'ShareOfInflow-SEIS'!B15</f>
         <v>7.6828779999999997</v>
       </c>
       <c r="C5" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="56">
-        <f>'ShareOfInflow-SEIS'!C14</f>
+        <f>'ShareOfInflow-SEIS'!C15</f>
         <v>0.2107804750717828</v>
       </c>
       <c r="H5" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="76">
+      <c r="I5" s="61">
         <v>0.30470849398294192</v>
       </c>
-      <c r="J5" s="76">
+      <c r="J5" s="61">
         <v>0.2822759668185536</v>
       </c>
-      <c r="K5" s="76">
+      <c r="K5" s="61">
         <v>0.29594578805935273</v>
       </c>
-      <c r="L5" s="76">
+      <c r="L5" s="61">
         <v>3.4116135062507304E-2</v>
       </c>
-      <c r="M5" s="76">
+      <c r="M5" s="61">
         <v>3.3181446430657784E-2</v>
       </c>
-      <c r="N5" s="76">
+      <c r="N5" s="61">
         <v>3.3181446430657784E-2</v>
       </c>
-      <c r="O5" s="76">
+      <c r="O5" s="61">
         <v>0.51407874751723337</v>
       </c>
-      <c r="P5" s="76">
+      <c r="P5" s="61">
         <v>0.51407874751723337</v>
       </c>
-      <c r="Q5" s="76">
+      <c r="Q5" s="61">
         <v>0.5004089262764343</v>
       </c>
-      <c r="R5" s="76">
+      <c r="R5" s="61">
         <v>0.17046383923355535</v>
       </c>
-      <c r="S5" s="76">
+      <c r="S5" s="61">
         <v>0.17046383923355535</v>
       </c>
-      <c r="T5" s="76">
+      <c r="T5" s="61">
         <v>0.17046383923355535</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
-        <f>'ShareOfInflow-SEIS'!A15</f>
+        <f>'ShareOfInflow-SEIS'!A16</f>
         <v>1,045–&gt;1,040</v>
       </c>
       <c r="B6" s="7">
-        <f>'ShareOfInflow-SEIS'!B15</f>
+        <f>'ShareOfInflow-SEIS'!B16</f>
         <v>7.3260519999999998</v>
       </c>
       <c r="C6" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="56">
-        <f>'ShareOfInflow-SEIS'!C15</f>
+        <f>'ShareOfInflow-SEIS'!C16</f>
         <v>0.16401734104046239</v>
       </c>
       <c r="H6" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="76">
+      <c r="I6" s="61">
         <v>0.29131652661064422</v>
       </c>
-      <c r="J6" s="76">
+      <c r="J6" s="61">
         <v>0.22625413801884389</v>
       </c>
-      <c r="K6" s="76">
+      <c r="K6" s="61">
         <v>0.26597911892029541</v>
       </c>
-      <c r="L6" s="76">
+      <c r="L6" s="61">
         <v>3.5523300229182576E-2</v>
       </c>
-      <c r="M6" s="76">
+      <c r="M6" s="61">
         <v>3.2722179781003308E-2</v>
       </c>
-      <c r="N6" s="76">
+      <c r="N6" s="61">
         <v>3.2849503437738729E-2</v>
       </c>
-      <c r="O6" s="76">
+      <c r="O6" s="61">
         <v>0.56022408963585435</v>
       </c>
-      <c r="P6" s="76">
+      <c r="P6" s="61">
         <v>0.56022408963585435</v>
       </c>
-      <c r="Q6" s="76">
+      <c r="Q6" s="61">
         <v>0.52037178507766746</v>
       </c>
-      <c r="R6" s="76">
+      <c r="R6" s="61">
         <v>0.18079959256429842</v>
       </c>
-      <c r="S6" s="76">
+      <c r="S6" s="61">
         <v>0.18079959256429842</v>
       </c>
-      <c r="T6" s="76">
+      <c r="T6" s="61">
         <v>0.18079959256429842</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
-        <f>'ShareOfInflow-SEIS'!A16</f>
+        <f>'ShareOfInflow-SEIS'!A17</f>
         <v>1,040–&gt;1,035</v>
       </c>
       <c r="B7" s="7">
-        <f>'ShareOfInflow-SEIS'!B16</f>
+        <f>'ShareOfInflow-SEIS'!B17</f>
         <v>6.977665</v>
       </c>
       <c r="C7" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="56">
-        <f>'ShareOfInflow-SEIS'!C16</f>
+        <f>'ShareOfInflow-SEIS'!C17</f>
         <v>0.15703090344521659</v>
       </c>
       <c r="H7" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="76">
+      <c r="I7" s="61">
         <v>0.3033707865168539</v>
       </c>
-      <c r="J7" s="76">
+      <c r="J7" s="61">
         <v>0.16401734104046239</v>
       </c>
-      <c r="K7" s="76">
+      <c r="K7" s="61">
         <v>0.25786516853932584</v>
       </c>
-      <c r="L7" s="76">
+      <c r="L7" s="61">
         <v>3.8342696629213475E-2</v>
       </c>
-      <c r="M7" s="76">
+      <c r="M7" s="61">
         <v>3.3381502890173408E-2</v>
       </c>
-      <c r="N7" s="76">
+      <c r="N7" s="61">
         <v>3.3426966292134833E-2</v>
       </c>
-      <c r="O7" s="76">
+      <c r="O7" s="61">
         <v>0.5898876404494382</v>
       </c>
-      <c r="P7" s="76">
+      <c r="P7" s="61">
         <v>0.60693641618497118</v>
       </c>
-      <c r="Q7" s="76">
+      <c r="Q7" s="61">
         <v>0.51839887640449445</v>
       </c>
-      <c r="R7" s="76">
+      <c r="R7" s="61">
         <v>0.19016853932584271</v>
       </c>
-      <c r="S7" s="76">
+      <c r="S7" s="61">
         <v>0.19566473988439309</v>
       </c>
-      <c r="T7" s="76">
+      <c r="T7" s="61">
         <v>0.19016853932584271</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
-        <f>'ShareOfInflow-SEIS'!A17</f>
+        <f>'ShareOfInflow-SEIS'!A18</f>
         <v>1,035–&gt;1,030</v>
       </c>
       <c r="B8" s="7">
-        <f>'ShareOfInflow-SEIS'!B17</f>
+        <f>'ShareOfInflow-SEIS'!B18</f>
         <v>6.6375080000000004</v>
       </c>
       <c r="C8" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="56">
-        <f>'ShareOfInflow-SEIS'!C17</f>
+        <f>'ShareOfInflow-SEIS'!C18</f>
         <v>0.15810629745422058</v>
       </c>
       <c r="H8" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="I8" s="76">
+      <c r="I8" s="61">
         <v>0.30804335424985735</v>
       </c>
-      <c r="J8" s="76">
+      <c r="J8" s="61">
         <v>0.15703090344521659</v>
       </c>
-      <c r="K8" s="76">
+      <c r="K8" s="61">
         <v>0.25506432056779532</v>
       </c>
-      <c r="L8" s="76">
+      <c r="L8" s="61">
         <v>3.8933257273245855E-2</v>
       </c>
-      <c r="M8" s="76">
+      <c r="M8" s="61">
         <v>3.2086352210557438E-2</v>
       </c>
-      <c r="N8" s="76">
+      <c r="N8" s="61">
         <v>3.3417122578737246E-2</v>
       </c>
-      <c r="O8" s="76">
+      <c r="O8" s="61">
         <v>0.59184255561893895</v>
       </c>
-      <c r="P8" s="76">
+      <c r="P8" s="61">
         <v>0.6118586426142244</v>
       </c>
-      <c r="Q8" s="76">
+      <c r="Q8" s="61">
         <v>0.51249445512346592</v>
       </c>
-      <c r="R8" s="76">
+      <c r="R8" s="61">
         <v>0.19195664575014262</v>
       </c>
-      <c r="S8" s="76">
+      <c r="S8" s="61">
         <v>0.19902410173000148</v>
       </c>
-      <c r="T8" s="76">
+      <c r="T8" s="61">
         <v>0.19902410173000148</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
-        <f>'ShareOfInflow-SEIS'!A18</f>
+        <f>'ShareOfInflow-SEIS'!A19</f>
         <v>1,030–1,025</v>
       </c>
       <c r="B9" s="7">
-        <f>'ShareOfInflow-SEIS'!B18</f>
+        <f>'ShareOfInflow-SEIS'!B19</f>
         <v>6.305377</v>
       </c>
       <c r="C9" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="56">
-        <f>'ShareOfInflow-SEIS'!C18</f>
+        <f>'ShareOfInflow-SEIS'!C19</f>
         <v>0.15950735956743767</v>
       </c>
       <c r="H9" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="76">
+      <c r="I9" s="61">
         <v>0.31286210892236382</v>
       </c>
-      <c r="J9" s="76">
+      <c r="J9" s="61">
         <v>0.15810629745422058</v>
       </c>
-      <c r="K9" s="76">
+      <c r="K9" s="61">
         <v>0.25803108808290154</v>
       </c>
-      <c r="L9" s="76">
+      <c r="L9" s="61">
         <v>3.9542294322132091E-2</v>
       </c>
-      <c r="M9" s="76">
+      <c r="M9" s="61">
         <v>3.2306089027839803E-2</v>
       </c>
-      <c r="N9" s="76">
+      <c r="N9" s="61">
         <v>3.3752775721687639E-2</v>
       </c>
-      <c r="O9" s="76">
+      <c r="O9" s="61">
         <v>0.59385863267670924</v>
       </c>
-      <c r="P9" s="76">
+      <c r="P9" s="61">
         <v>0.61039154384397798</v>
       </c>
-      <c r="Q9" s="76">
+      <c r="Q9" s="61">
         <v>0.50999259807549968</v>
       </c>
-      <c r="R9" s="76">
+      <c r="R9" s="61">
         <v>0.19380069524913096</v>
       </c>
-      <c r="S9" s="76">
+      <c r="S9" s="61">
         <v>0.19919606967396158</v>
       </c>
-      <c r="T9" s="76">
+      <c r="T9" s="61">
         <v>0.19807549962990378</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
-        <f>'ShareOfInflow-SEIS'!A19</f>
+        <f>'ShareOfInflow-SEIS'!A20</f>
         <v>&lt;1,025–1,000</v>
       </c>
       <c r="B10" s="7">
-        <f>'ShareOfInflow-SEIS'!B19</f>
+        <f>'ShareOfInflow-SEIS'!B20</f>
         <v>5.981122</v>
       </c>
       <c r="C10" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="56">
-        <f>'ShareOfInflow-SEIS'!C19</f>
+        <f>'ShareOfInflow-SEIS'!C20</f>
         <v>0.1620384498016478</v>
       </c>
       <c r="H10" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="I10" s="76">
+      <c r="I10" s="61">
         <v>0.31788079470198671</v>
       </c>
-      <c r="J10" s="76">
+      <c r="J10" s="61">
         <v>0.15950735956743767</v>
       </c>
-      <c r="K10" s="76">
+      <c r="K10" s="61">
         <v>0.26119181737325819</v>
       </c>
-      <c r="L10" s="76">
+      <c r="L10" s="61">
         <v>4.0176600441501099E-2</v>
       </c>
-      <c r="M10" s="76">
+      <c r="M10" s="61">
         <v>3.2592370081105437E-2</v>
       </c>
-      <c r="N10" s="76">
+      <c r="N10" s="61">
         <v>3.4094278090720423E-2</v>
       </c>
-      <c r="O10" s="76">
+      <c r="O10" s="61">
         <v>0.59602649006622532</v>
       </c>
-      <c r="P10" s="76">
+      <c r="P10" s="61">
         <v>0.60829077801141496</v>
       </c>
-      <c r="Q10" s="76">
+      <c r="Q10" s="61">
         <v>0.50770827156833676</v>
       </c>
-      <c r="R10" s="76">
+      <c r="R10" s="61">
         <v>0.19558498896247239</v>
       </c>
-      <c r="S10" s="76">
+      <c r="S10" s="61">
         <v>0.19960949234004208</v>
       </c>
-      <c r="T10" s="76">
+      <c r="T10" s="61">
         <v>0.19700563296768453</v>
       </c>
     </row>
@@ -3360,7 +3243,7 @@
         <v>10.857008</v>
       </c>
       <c r="C11" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D11" t="str">
@@ -3368,46 +3251,46 @@
         <v>Arizona</v>
       </c>
       <c r="E11" s="56">
-        <f>'ShareOfInflow-SEIS'!H12</f>
+        <f>'ShareOfInflow-SEIS'!H13</f>
         <v>0.29594578805935273</v>
       </c>
       <c r="H11" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="76">
+      <c r="I11" s="61">
         <v>0.28817541111981204</v>
       </c>
-      <c r="J11" s="76">
+      <c r="J11" s="61">
         <v>0.2107804750717828</v>
       </c>
-      <c r="K11" s="76">
+      <c r="K11" s="61">
         <v>0.25815713912816496</v>
       </c>
-      <c r="L11" s="76">
+      <c r="L11" s="61">
         <v>3.5891412163925863E-2</v>
       </c>
-      <c r="M11" s="76">
+      <c r="M11" s="61">
         <v>3.2759070738710518E-2</v>
       </c>
-      <c r="N11" s="76">
+      <c r="N11" s="61">
         <v>3.2628556512659883E-2</v>
       </c>
-      <c r="O11" s="76">
+      <c r="O11" s="61">
         <v>0.57426259462281393</v>
       </c>
-      <c r="P11" s="76">
+      <c r="P11" s="61">
         <v>0.57426259462281393</v>
       </c>
-      <c r="Q11" s="76">
+      <c r="Q11" s="61">
         <v>0.52701644479248244</v>
       </c>
-      <c r="R11" s="76">
+      <c r="R11" s="61">
         <v>0.18219785956669277</v>
       </c>
-      <c r="S11" s="76">
+      <c r="S11" s="61">
         <v>0.18219785956669277</v>
       </c>
-      <c r="T11" s="76">
+      <c r="T11" s="61">
         <v>0.18219785956669277</v>
       </c>
     </row>
@@ -3421,7 +3304,7 @@
         <v>9.6009879999900001</v>
       </c>
       <c r="C12" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D12" t="str">
@@ -3429,46 +3312,46 @@
         <v>Arizona</v>
       </c>
       <c r="E12" s="56">
-        <f>'ShareOfInflow-SEIS'!H13</f>
+        <f>'ShareOfInflow-SEIS'!H14</f>
         <v>0.26597911892029541</v>
       </c>
       <c r="H12" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="I12" s="76">
+      <c r="I12" s="61">
         <v>0.31877394636015327</v>
       </c>
-      <c r="J12" s="76">
+      <c r="J12" s="61">
         <v>0.1620384498016478</v>
       </c>
-      <c r="K12" s="76">
+      <c r="K12" s="61">
         <v>0.25790424570912374</v>
       </c>
-      <c r="L12" s="76">
+      <c r="L12" s="61">
         <v>4.1379310344827586E-2</v>
       </c>
-      <c r="M12" s="76">
+      <c r="M12" s="61">
         <v>3.3109551418980768E-2</v>
       </c>
-      <c r="N12" s="76">
+      <c r="N12" s="61">
         <v>3.4778681120144532E-2</v>
       </c>
-      <c r="O12" s="76">
+      <c r="O12" s="61">
         <v>0.62068965517241392</v>
       </c>
-      <c r="P12" s="76">
+      <c r="P12" s="61">
         <v>0.61794324076899609</v>
       </c>
-      <c r="Q12" s="76">
+      <c r="Q12" s="61">
         <v>0.52288467329117749</v>
       </c>
-      <c r="R12" s="76">
+      <c r="R12" s="61">
         <v>0.18773946360153257</v>
       </c>
-      <c r="S12" s="76">
+      <c r="S12" s="61">
         <v>0.18690875801037535</v>
       </c>
-      <c r="T12" s="76">
+      <c r="T12" s="61">
         <v>0.18443239987955437</v>
       </c>
     </row>
@@ -3482,7 +3365,7 @@
         <v>7.6828779999999997</v>
       </c>
       <c r="C13" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D13" t="str">
@@ -3490,7 +3373,7 @@
         <v>Arizona</v>
       </c>
       <c r="E13" s="56">
-        <f>'ShareOfInflow-SEIS'!H14</f>
+        <f>'ShareOfInflow-SEIS'!H15</f>
         <v>0.25815713912816496</v>
       </c>
     </row>
@@ -3504,7 +3387,7 @@
         <v>7.3260519999999998</v>
       </c>
       <c r="C14" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D14" t="str">
@@ -3512,7 +3395,7 @@
         <v>Arizona</v>
       </c>
       <c r="E14" s="56">
-        <f>'ShareOfInflow-SEIS'!H15</f>
+        <f>'ShareOfInflow-SEIS'!H16</f>
         <v>0.25786516853932584</v>
       </c>
     </row>
@@ -3526,7 +3409,7 @@
         <v>6.977665</v>
       </c>
       <c r="C15" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D15" t="str">
@@ -3534,7 +3417,7 @@
         <v>Arizona</v>
       </c>
       <c r="E15" s="56">
-        <f>'ShareOfInflow-SEIS'!H16</f>
+        <f>'ShareOfInflow-SEIS'!H17</f>
         <v>0.25506432056779532</v>
       </c>
     </row>
@@ -3548,7 +3431,7 @@
         <v>6.6375080000000004</v>
       </c>
       <c r="C16" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D16" t="str">
@@ -3556,7 +3439,7 @@
         <v>Arizona</v>
       </c>
       <c r="E16" s="56">
-        <f>'ShareOfInflow-SEIS'!H17</f>
+        <f>'ShareOfInflow-SEIS'!H18</f>
         <v>0.25803108808290154</v>
       </c>
     </row>
@@ -3570,7 +3453,7 @@
         <v>6.305377</v>
       </c>
       <c r="C17" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D17" t="str">
@@ -3578,7 +3461,7 @@
         <v>Arizona</v>
       </c>
       <c r="E17" s="56">
-        <f>'ShareOfInflow-SEIS'!H18</f>
+        <f>'ShareOfInflow-SEIS'!H19</f>
         <v>0.26119181737325819</v>
       </c>
     </row>
@@ -3592,7 +3475,7 @@
         <v>5.981122</v>
       </c>
       <c r="C18" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D18" t="str">
@@ -3600,7 +3483,7 @@
         <v>Arizona</v>
       </c>
       <c r="E18" s="56">
-        <f>'ShareOfInflow-SEIS'!H19</f>
+        <f>'ShareOfInflow-SEIS'!H20</f>
         <v>0.25790424570912374</v>
       </c>
     </row>
@@ -3614,7 +3497,7 @@
         <v>10.857008</v>
       </c>
       <c r="C19" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D19" t="str">
@@ -3622,7 +3505,7 @@
         <v>Arizona</v>
       </c>
       <c r="E19" s="56">
-        <f>'ShareOfInflow-SEIS'!M12</f>
+        <f>'ShareOfInflow-SEIS'!M13</f>
         <v>0.30470849398294192</v>
       </c>
     </row>
@@ -3636,7 +3519,7 @@
         <v>9.6009879999900001</v>
       </c>
       <c r="C20" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D20" t="str">
@@ -3644,7 +3527,7 @@
         <v>Arizona</v>
       </c>
       <c r="E20" s="56">
-        <f>'ShareOfInflow-SEIS'!M13</f>
+        <f>'ShareOfInflow-SEIS'!M14</f>
         <v>0.29131652661064422</v>
       </c>
     </row>
@@ -3658,7 +3541,7 @@
         <v>7.6828779999999997</v>
       </c>
       <c r="C21" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D21" t="str">
@@ -3666,7 +3549,7 @@
         <v>Arizona</v>
       </c>
       <c r="E21" s="56">
-        <f>'ShareOfInflow-SEIS'!M14</f>
+        <f>'ShareOfInflow-SEIS'!M15</f>
         <v>0.28817541111981204</v>
       </c>
     </row>
@@ -3680,7 +3563,7 @@
         <v>7.3260519999999998</v>
       </c>
       <c r="C22" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D22" t="str">
@@ -3688,7 +3571,7 @@
         <v>Arizona</v>
       </c>
       <c r="E22" s="56">
-        <f>'ShareOfInflow-SEIS'!M15</f>
+        <f>'ShareOfInflow-SEIS'!M16</f>
         <v>0.3033707865168539</v>
       </c>
     </row>
@@ -3702,7 +3585,7 @@
         <v>6.977665</v>
       </c>
       <c r="C23" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D23" t="str">
@@ -3710,7 +3593,7 @@
         <v>Arizona</v>
       </c>
       <c r="E23" s="56">
-        <f>'ShareOfInflow-SEIS'!M16</f>
+        <f>'ShareOfInflow-SEIS'!M17</f>
         <v>0.30804335424985735</v>
       </c>
     </row>
@@ -3724,7 +3607,7 @@
         <v>6.6375080000000004</v>
       </c>
       <c r="C24" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D24" t="str">
@@ -3732,7 +3615,7 @@
         <v>Arizona</v>
       </c>
       <c r="E24" s="56">
-        <f>'ShareOfInflow-SEIS'!M17</f>
+        <f>'ShareOfInflow-SEIS'!M18</f>
         <v>0.31286210892236382</v>
       </c>
     </row>
@@ -3746,7 +3629,7 @@
         <v>6.305377</v>
       </c>
       <c r="C25" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D25" t="str">
@@ -3754,7 +3637,7 @@
         <v>Arizona</v>
       </c>
       <c r="E25" s="56">
-        <f>'ShareOfInflow-SEIS'!M18</f>
+        <f>'ShareOfInflow-SEIS'!M19</f>
         <v>0.31788079470198671</v>
       </c>
     </row>
@@ -3768,7 +3651,7 @@
         <v>5.981122</v>
       </c>
       <c r="C26" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D26" t="str">
@@ -3776,7 +3659,7 @@
         <v>Arizona</v>
       </c>
       <c r="E26" s="56">
-        <f>'ShareOfInflow-SEIS'!M19</f>
+        <f>'ShareOfInflow-SEIS'!M20</f>
         <v>0.31877394636015327</v>
       </c>
     </row>
@@ -3790,14 +3673,14 @@
         <v>10.857008</v>
       </c>
       <c r="C27" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D27" t="s">
         <v>19</v>
       </c>
       <c r="E27" s="56">
-        <f>'ShareOfInflow-SEIS'!D12</f>
+        <f>'ShareOfInflow-SEIS'!D13</f>
         <v>3.3181446430657784E-2</v>
       </c>
     </row>
@@ -3811,14 +3694,14 @@
         <v>9.6009879999900001</v>
       </c>
       <c r="C28" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D28" t="s">
         <v>19</v>
       </c>
       <c r="E28" s="56">
-        <f>'ShareOfInflow-SEIS'!D13</f>
+        <f>'ShareOfInflow-SEIS'!D14</f>
         <v>3.2722179781003308E-2</v>
       </c>
     </row>
@@ -3832,14 +3715,14 @@
         <v>7.6828779999999997</v>
       </c>
       <c r="C29" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D29" t="s">
         <v>19</v>
       </c>
       <c r="E29" s="56">
-        <f>'ShareOfInflow-SEIS'!D14</f>
+        <f>'ShareOfInflow-SEIS'!D15</f>
         <v>3.2759070738710518E-2</v>
       </c>
     </row>
@@ -3853,14 +3736,14 @@
         <v>7.3260519999999998</v>
       </c>
       <c r="C30" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D30" t="s">
         <v>19</v>
       </c>
       <c r="E30" s="56">
-        <f>'ShareOfInflow-SEIS'!D15</f>
+        <f>'ShareOfInflow-SEIS'!D16</f>
         <v>3.3381502890173408E-2</v>
       </c>
     </row>
@@ -3874,14 +3757,14 @@
         <v>6.977665</v>
       </c>
       <c r="C31" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D31" t="s">
         <v>19</v>
       </c>
       <c r="E31" s="56">
-        <f>'ShareOfInflow-SEIS'!D16</f>
+        <f>'ShareOfInflow-SEIS'!D17</f>
         <v>3.2086352210557438E-2</v>
       </c>
     </row>
@@ -3895,14 +3778,14 @@
         <v>6.6375080000000004</v>
       </c>
       <c r="C32" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D32" t="s">
         <v>19</v>
       </c>
       <c r="E32" s="56">
-        <f>'ShareOfInflow-SEIS'!D17</f>
+        <f>'ShareOfInflow-SEIS'!D18</f>
         <v>3.2306089027839803E-2</v>
       </c>
     </row>
@@ -3916,14 +3799,14 @@
         <v>6.305377</v>
       </c>
       <c r="C33" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D33" t="s">
         <v>19</v>
       </c>
       <c r="E33" s="56">
-        <f>'ShareOfInflow-SEIS'!D18</f>
+        <f>'ShareOfInflow-SEIS'!D19</f>
         <v>3.2592370081105437E-2</v>
       </c>
     </row>
@@ -3937,14 +3820,14 @@
         <v>5.981122</v>
       </c>
       <c r="C34" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D34" t="s">
         <v>19</v>
       </c>
       <c r="E34" s="56">
-        <f>'ShareOfInflow-SEIS'!D19</f>
+        <f>'ShareOfInflow-SEIS'!D20</f>
         <v>3.3109551418980768E-2</v>
       </c>
     </row>
@@ -3958,14 +3841,14 @@
         <v>10.857008</v>
       </c>
       <c r="C35" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D35" t="s">
         <v>19</v>
       </c>
       <c r="E35" s="56">
-        <f>'ShareOfInflow-SEIS'!I12</f>
+        <f>'ShareOfInflow-SEIS'!I13</f>
         <v>3.3181446430657784E-2</v>
       </c>
     </row>
@@ -3979,14 +3862,14 @@
         <v>9.6009879999900001</v>
       </c>
       <c r="C36" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D36" t="s">
         <v>19</v>
       </c>
       <c r="E36" s="56">
-        <f>'ShareOfInflow-SEIS'!I13</f>
+        <f>'ShareOfInflow-SEIS'!I14</f>
         <v>3.2849503437738729E-2</v>
       </c>
     </row>
@@ -4000,14 +3883,14 @@
         <v>7.6828779999999997</v>
       </c>
       <c r="C37" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D37" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="56">
-        <f>'ShareOfInflow-SEIS'!I14</f>
+        <f>'ShareOfInflow-SEIS'!I15</f>
         <v>3.2628556512659883E-2</v>
       </c>
     </row>
@@ -4021,14 +3904,14 @@
         <v>7.3260519999999998</v>
       </c>
       <c r="C38" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D38" t="s">
         <v>19</v>
       </c>
       <c r="E38" s="56">
-        <f>'ShareOfInflow-SEIS'!I15</f>
+        <f>'ShareOfInflow-SEIS'!I16</f>
         <v>3.3426966292134833E-2</v>
       </c>
     </row>
@@ -4042,14 +3925,14 @@
         <v>6.977665</v>
       </c>
       <c r="C39" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D39" t="s">
         <v>19</v>
       </c>
       <c r="E39" s="56">
-        <f>'ShareOfInflow-SEIS'!I16</f>
+        <f>'ShareOfInflow-SEIS'!I17</f>
         <v>3.3417122578737246E-2</v>
       </c>
     </row>
@@ -4063,14 +3946,14 @@
         <v>6.6375080000000004</v>
       </c>
       <c r="C40" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D40" t="s">
         <v>19</v>
       </c>
       <c r="E40" s="56">
-        <f>'ShareOfInflow-SEIS'!I17</f>
+        <f>'ShareOfInflow-SEIS'!I18</f>
         <v>3.3752775721687639E-2</v>
       </c>
     </row>
@@ -4084,14 +3967,14 @@
         <v>6.305377</v>
       </c>
       <c r="C41" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D41" t="s">
         <v>19</v>
       </c>
       <c r="E41" s="56">
-        <f>'ShareOfInflow-SEIS'!I18</f>
+        <f>'ShareOfInflow-SEIS'!I19</f>
         <v>3.4094278090720423E-2</v>
       </c>
     </row>
@@ -4105,14 +3988,14 @@
         <v>5.981122</v>
       </c>
       <c r="C42" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D42" t="s">
         <v>19</v>
       </c>
       <c r="E42" s="56">
-        <f>'ShareOfInflow-SEIS'!I19</f>
+        <f>'ShareOfInflow-SEIS'!I20</f>
         <v>3.4778681120144532E-2</v>
       </c>
     </row>
@@ -4126,14 +4009,14 @@
         <v>10.857008</v>
       </c>
       <c r="C43" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D43" t="s">
         <v>19</v>
       </c>
       <c r="E43" s="56">
-        <f>'ShareOfInflow-SEIS'!N12</f>
+        <f>'ShareOfInflow-SEIS'!N13</f>
         <v>3.4116135062507304E-2</v>
       </c>
     </row>
@@ -4147,14 +4030,14 @@
         <v>9.6009879999900001</v>
       </c>
       <c r="C44" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D44" t="s">
         <v>19</v>
       </c>
       <c r="E44" s="56">
-        <f>'ShareOfInflow-SEIS'!N13</f>
+        <f>'ShareOfInflow-SEIS'!N14</f>
         <v>3.5523300229182576E-2</v>
       </c>
     </row>
@@ -4168,14 +4051,14 @@
         <v>7.6828779999999997</v>
       </c>
       <c r="C45" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D45" t="s">
         <v>19</v>
       </c>
       <c r="E45" s="56">
-        <f>'ShareOfInflow-SEIS'!N14</f>
+        <f>'ShareOfInflow-SEIS'!N15</f>
         <v>3.5891412163925863E-2</v>
       </c>
     </row>
@@ -4189,14 +4072,14 @@
         <v>7.3260519999999998</v>
       </c>
       <c r="C46" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D46" t="s">
         <v>19</v>
       </c>
       <c r="E46" s="56">
-        <f>'ShareOfInflow-SEIS'!N15</f>
+        <f>'ShareOfInflow-SEIS'!N16</f>
         <v>3.8342696629213475E-2</v>
       </c>
     </row>
@@ -4210,14 +4093,14 @@
         <v>6.977665</v>
       </c>
       <c r="C47" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D47" t="s">
         <v>19</v>
       </c>
       <c r="E47" s="56">
-        <f>'ShareOfInflow-SEIS'!N16</f>
+        <f>'ShareOfInflow-SEIS'!N17</f>
         <v>3.8933257273245855E-2</v>
       </c>
     </row>
@@ -4231,14 +4114,14 @@
         <v>6.6375080000000004</v>
       </c>
       <c r="C48" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D48" t="s">
         <v>19</v>
       </c>
       <c r="E48" s="56">
-        <f>'ShareOfInflow-SEIS'!N17</f>
+        <f>'ShareOfInflow-SEIS'!N18</f>
         <v>3.9542294322132091E-2</v>
       </c>
     </row>
@@ -4252,14 +4135,14 @@
         <v>6.305377</v>
       </c>
       <c r="C49" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D49" t="s">
         <v>19</v>
       </c>
       <c r="E49" s="56">
-        <f>'ShareOfInflow-SEIS'!N18</f>
+        <f>'ShareOfInflow-SEIS'!N19</f>
         <v>4.0176600441501099E-2</v>
       </c>
     </row>
@@ -4273,14 +4156,14 @@
         <v>5.981122</v>
       </c>
       <c r="C50" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D50" t="s">
         <v>19</v>
       </c>
       <c r="E50" s="56">
-        <f>'ShareOfInflow-SEIS'!N19</f>
+        <f>'ShareOfInflow-SEIS'!N20</f>
         <v>4.1379310344827586E-2</v>
       </c>
     </row>
@@ -4294,14 +4177,14 @@
         <v>10.857008</v>
       </c>
       <c r="C51" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D51" t="s">
         <v>20</v>
       </c>
       <c r="E51" s="56">
-        <f>'ShareOfInflow-SEIS'!E12</f>
+        <f>'ShareOfInflow-SEIS'!E13</f>
         <v>0.51407874751723337</v>
       </c>
     </row>
@@ -4315,14 +4198,14 @@
         <v>9.6009879999900001</v>
       </c>
       <c r="C52" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D52" t="s">
         <v>20</v>
       </c>
       <c r="E52" s="56">
-        <f>'ShareOfInflow-SEIS'!E13</f>
+        <f>'ShareOfInflow-SEIS'!E14</f>
         <v>0.56022408963585435</v>
       </c>
     </row>
@@ -4336,14 +4219,14 @@
         <v>7.6828779999999997</v>
       </c>
       <c r="C53" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D53" t="s">
         <v>20</v>
       </c>
       <c r="E53" s="56">
-        <f>'ShareOfInflow-SEIS'!E14</f>
+        <f>'ShareOfInflow-SEIS'!E15</f>
         <v>0.57426259462281393</v>
       </c>
     </row>
@@ -4357,14 +4240,14 @@
         <v>7.3260519999999998</v>
       </c>
       <c r="C54" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D54" t="s">
         <v>20</v>
       </c>
       <c r="E54" s="56">
-        <f>'ShareOfInflow-SEIS'!E15</f>
+        <f>'ShareOfInflow-SEIS'!E16</f>
         <v>0.60693641618497118</v>
       </c>
     </row>
@@ -4378,14 +4261,14 @@
         <v>6.977665</v>
       </c>
       <c r="C55" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D55" t="s">
         <v>20</v>
       </c>
       <c r="E55" s="56">
-        <f>'ShareOfInflow-SEIS'!E16</f>
+        <f>'ShareOfInflow-SEIS'!E17</f>
         <v>0.6118586426142244</v>
       </c>
     </row>
@@ -4399,14 +4282,14 @@
         <v>6.6375080000000004</v>
       </c>
       <c r="C56" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D56" t="s">
         <v>20</v>
       </c>
       <c r="E56" s="56">
-        <f>'ShareOfInflow-SEIS'!E17</f>
+        <f>'ShareOfInflow-SEIS'!E18</f>
         <v>0.61039154384397798</v>
       </c>
     </row>
@@ -4420,14 +4303,14 @@
         <v>6.305377</v>
       </c>
       <c r="C57" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D57" t="s">
         <v>20</v>
       </c>
       <c r="E57" s="56">
-        <f>'ShareOfInflow-SEIS'!E18</f>
+        <f>'ShareOfInflow-SEIS'!E19</f>
         <v>0.60829077801141496</v>
       </c>
     </row>
@@ -4441,14 +4324,14 @@
         <v>5.981122</v>
       </c>
       <c r="C58" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D58" t="s">
         <v>20</v>
       </c>
       <c r="E58" s="56">
-        <f>'ShareOfInflow-SEIS'!E19</f>
+        <f>'ShareOfInflow-SEIS'!E20</f>
         <v>0.61794324076899609</v>
       </c>
     </row>
@@ -4462,14 +4345,14 @@
         <v>10.857008</v>
       </c>
       <c r="C59" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D59" t="s">
         <v>20</v>
       </c>
       <c r="E59" s="56">
-        <f>'ShareOfInflow-SEIS'!J12</f>
+        <f>'ShareOfInflow-SEIS'!J13</f>
         <v>0.5004089262764343</v>
       </c>
     </row>
@@ -4483,14 +4366,14 @@
         <v>9.6009879999900001</v>
       </c>
       <c r="C60" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D60" t="s">
         <v>20</v>
       </c>
       <c r="E60" s="56">
-        <f>'ShareOfInflow-SEIS'!J13</f>
+        <f>'ShareOfInflow-SEIS'!J14</f>
         <v>0.52037178507766746</v>
       </c>
     </row>
@@ -4504,14 +4387,14 @@
         <v>7.6828779999999997</v>
       </c>
       <c r="C61" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D61" t="s">
         <v>20</v>
       </c>
       <c r="E61" s="56">
-        <f>'ShareOfInflow-SEIS'!J14</f>
+        <f>'ShareOfInflow-SEIS'!J15</f>
         <v>0.52701644479248244</v>
       </c>
     </row>
@@ -4525,14 +4408,14 @@
         <v>7.3260519999999998</v>
       </c>
       <c r="C62" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D62" t="s">
         <v>20</v>
       </c>
       <c r="E62" s="56">
-        <f>'ShareOfInflow-SEIS'!J15</f>
+        <f>'ShareOfInflow-SEIS'!J16</f>
         <v>0.51839887640449445</v>
       </c>
     </row>
@@ -4546,14 +4429,14 @@
         <v>6.977665</v>
       </c>
       <c r="C63" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D63" t="s">
         <v>20</v>
       </c>
       <c r="E63" s="56">
-        <f>'ShareOfInflow-SEIS'!J16</f>
+        <f>'ShareOfInflow-SEIS'!J17</f>
         <v>0.51249445512346592</v>
       </c>
     </row>
@@ -4567,14 +4450,14 @@
         <v>6.6375080000000004</v>
       </c>
       <c r="C64" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D64" t="s">
         <v>20</v>
       </c>
       <c r="E64" s="56">
-        <f>'ShareOfInflow-SEIS'!J17</f>
+        <f>'ShareOfInflow-SEIS'!J18</f>
         <v>0.50999259807549968</v>
       </c>
     </row>
@@ -4588,14 +4471,14 @@
         <v>6.305377</v>
       </c>
       <c r="C65" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D65" t="s">
         <v>20</v>
       </c>
       <c r="E65" s="56">
-        <f>'ShareOfInflow-SEIS'!J18</f>
+        <f>'ShareOfInflow-SEIS'!J19</f>
         <v>0.50770827156833676</v>
       </c>
     </row>
@@ -4609,14 +4492,14 @@
         <v>5.981122</v>
       </c>
       <c r="C66" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D66" t="s">
         <v>20</v>
       </c>
       <c r="E66" s="56">
-        <f>'ShareOfInflow-SEIS'!J19</f>
+        <f>'ShareOfInflow-SEIS'!J20</f>
         <v>0.52288467329117749</v>
       </c>
     </row>
@@ -4630,14 +4513,14 @@
         <v>10.857008</v>
       </c>
       <c r="C67" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D67" t="s">
         <v>20</v>
       </c>
       <c r="E67" s="56">
-        <f>'ShareOfInflow-SEIS'!O12</f>
+        <f>'ShareOfInflow-SEIS'!O13</f>
         <v>0.51407874751723337</v>
       </c>
     </row>
@@ -4651,14 +4534,14 @@
         <v>9.6009879999900001</v>
       </c>
       <c r="C68" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D68" t="s">
         <v>20</v>
       </c>
       <c r="E68" s="56">
-        <f>'ShareOfInflow-SEIS'!O13</f>
+        <f>'ShareOfInflow-SEIS'!O14</f>
         <v>0.56022408963585435</v>
       </c>
     </row>
@@ -4672,14 +4555,14 @@
         <v>7.6828779999999997</v>
       </c>
       <c r="C69" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D69" t="s">
         <v>20</v>
       </c>
       <c r="E69" s="56">
-        <f>'ShareOfInflow-SEIS'!O14</f>
+        <f>'ShareOfInflow-SEIS'!O15</f>
         <v>0.57426259462281393</v>
       </c>
     </row>
@@ -4693,14 +4576,14 @@
         <v>7.3260519999999998</v>
       </c>
       <c r="C70" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D70" t="s">
         <v>20</v>
       </c>
       <c r="E70" s="56">
-        <f>'ShareOfInflow-SEIS'!O15</f>
+        <f>'ShareOfInflow-SEIS'!O16</f>
         <v>0.5898876404494382</v>
       </c>
     </row>
@@ -4714,14 +4597,14 @@
         <v>6.977665</v>
       </c>
       <c r="C71" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D71" t="s">
         <v>20</v>
       </c>
       <c r="E71" s="56">
-        <f>'ShareOfInflow-SEIS'!O16</f>
+        <f>'ShareOfInflow-SEIS'!O17</f>
         <v>0.59184255561893895</v>
       </c>
     </row>
@@ -4735,14 +4618,14 @@
         <v>6.6375080000000004</v>
       </c>
       <c r="C72" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D72" t="s">
         <v>20</v>
       </c>
       <c r="E72" s="56">
-        <f>'ShareOfInflow-SEIS'!O17</f>
+        <f>'ShareOfInflow-SEIS'!O18</f>
         <v>0.59385863267670924</v>
       </c>
     </row>
@@ -4756,14 +4639,14 @@
         <v>6.305377</v>
       </c>
       <c r="C73" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D73" t="s">
         <v>20</v>
       </c>
       <c r="E73" s="56">
-        <f>'ShareOfInflow-SEIS'!O18</f>
+        <f>'ShareOfInflow-SEIS'!O19</f>
         <v>0.59602649006622532</v>
       </c>
     </row>
@@ -4777,14 +4660,14 @@
         <v>5.981122</v>
       </c>
       <c r="C74" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D74" t="s">
         <v>20</v>
       </c>
       <c r="E74" s="56">
-        <f>'ShareOfInflow-SEIS'!O19</f>
+        <f>'ShareOfInflow-SEIS'!O20</f>
         <v>0.62068965517241392</v>
       </c>
     </row>
@@ -4798,14 +4681,14 @@
         <v>10.857008</v>
       </c>
       <c r="C75" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D75" t="s">
         <v>4</v>
       </c>
       <c r="E75" s="56">
-        <f>'ShareOfInflow-SEIS'!F12</f>
+        <f>'ShareOfInflow-SEIS'!F13</f>
         <v>0.17046383923355535</v>
       </c>
     </row>
@@ -4819,14 +4702,14 @@
         <v>9.6009879999900001</v>
       </c>
       <c r="C76" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D76" t="s">
         <v>4</v>
       </c>
       <c r="E76" s="56">
-        <f>'ShareOfInflow-SEIS'!F13</f>
+        <f>'ShareOfInflow-SEIS'!F14</f>
         <v>0.18079959256429842</v>
       </c>
     </row>
@@ -4840,14 +4723,14 @@
         <v>7.6828779999999997</v>
       </c>
       <c r="C77" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D77" t="s">
         <v>4</v>
       </c>
       <c r="E77" s="56">
-        <f>'ShareOfInflow-SEIS'!F14</f>
+        <f>'ShareOfInflow-SEIS'!F15</f>
         <v>0.18219785956669277</v>
       </c>
     </row>
@@ -4861,14 +4744,14 @@
         <v>7.3260519999999998</v>
       </c>
       <c r="C78" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D78" t="s">
         <v>4</v>
       </c>
       <c r="E78" s="56">
-        <f>'ShareOfInflow-SEIS'!F15</f>
+        <f>'ShareOfInflow-SEIS'!F16</f>
         <v>0.19566473988439309</v>
       </c>
     </row>
@@ -4882,14 +4765,14 @@
         <v>6.977665</v>
       </c>
       <c r="C79" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D79" t="s">
         <v>4</v>
       </c>
       <c r="E79" s="56">
-        <f>'ShareOfInflow-SEIS'!F16</f>
+        <f>'ShareOfInflow-SEIS'!F17</f>
         <v>0.19902410173000148</v>
       </c>
     </row>
@@ -4903,14 +4786,14 @@
         <v>6.6375080000000004</v>
       </c>
       <c r="C80" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D80" t="s">
         <v>4</v>
       </c>
       <c r="E80" s="56">
-        <f>'ShareOfInflow-SEIS'!F17</f>
+        <f>'ShareOfInflow-SEIS'!F18</f>
         <v>0.19919606967396158</v>
       </c>
     </row>
@@ -4924,14 +4807,14 @@
         <v>6.305377</v>
       </c>
       <c r="C81" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D81" t="s">
         <v>4</v>
       </c>
       <c r="E81" s="56">
-        <f>'ShareOfInflow-SEIS'!F18</f>
+        <f>'ShareOfInflow-SEIS'!F19</f>
         <v>0.19960949234004208</v>
       </c>
     </row>
@@ -4945,14 +4828,14 @@
         <v>5.981122</v>
       </c>
       <c r="C82" t="str">
-        <f>'ShareOfInflow-SEIS'!$C$10</f>
+        <f>'ShareOfInflow-SEIS'!$C$11</f>
         <v>Alternative 1 - Priority</v>
       </c>
       <c r="D82" t="s">
         <v>4</v>
       </c>
       <c r="E82" s="56">
-        <f>'ShareOfInflow-SEIS'!F19</f>
+        <f>'ShareOfInflow-SEIS'!F20</f>
         <v>0.18690875801037535</v>
       </c>
     </row>
@@ -4966,14 +4849,14 @@
         <v>10.857008</v>
       </c>
       <c r="C83" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D83" t="s">
         <v>4</v>
       </c>
       <c r="E83" s="56">
-        <f>'ShareOfInflow-SEIS'!K12</f>
+        <f>'ShareOfInflow-SEIS'!K13</f>
         <v>0.17046383923355535</v>
       </c>
     </row>
@@ -4987,14 +4870,14 @@
         <v>9.6009879999900001</v>
       </c>
       <c r="C84" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D84" t="s">
         <v>4</v>
       </c>
       <c r="E84" s="56">
-        <f>'ShareOfInflow-SEIS'!K13</f>
+        <f>'ShareOfInflow-SEIS'!K14</f>
         <v>0.18079959256429842</v>
       </c>
     </row>
@@ -5008,14 +4891,14 @@
         <v>7.6828779999999997</v>
       </c>
       <c r="C85" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D85" t="s">
         <v>4</v>
       </c>
       <c r="E85" s="56">
-        <f>'ShareOfInflow-SEIS'!K14</f>
+        <f>'ShareOfInflow-SEIS'!K15</f>
         <v>0.18219785956669277</v>
       </c>
     </row>
@@ -5029,14 +4912,14 @@
         <v>7.3260519999999998</v>
       </c>
       <c r="C86" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D86" t="s">
         <v>4</v>
       </c>
       <c r="E86" s="56">
-        <f>'ShareOfInflow-SEIS'!K15</f>
+        <f>'ShareOfInflow-SEIS'!K16</f>
         <v>0.19016853932584271</v>
       </c>
     </row>
@@ -5050,14 +4933,14 @@
         <v>6.977665</v>
       </c>
       <c r="C87" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D87" t="s">
         <v>4</v>
       </c>
       <c r="E87" s="56">
-        <f>'ShareOfInflow-SEIS'!K16</f>
+        <f>'ShareOfInflow-SEIS'!K17</f>
         <v>0.19902410173000148</v>
       </c>
     </row>
@@ -5071,14 +4954,14 @@
         <v>6.6375080000000004</v>
       </c>
       <c r="C88" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D88" t="s">
         <v>4</v>
       </c>
       <c r="E88" s="56">
-        <f>'ShareOfInflow-SEIS'!K17</f>
+        <f>'ShareOfInflow-SEIS'!K18</f>
         <v>0.19807549962990378</v>
       </c>
     </row>
@@ -5092,14 +4975,14 @@
         <v>6.305377</v>
       </c>
       <c r="C89" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D89" t="s">
         <v>4</v>
       </c>
       <c r="E89" s="56">
-        <f>'ShareOfInflow-SEIS'!K18</f>
+        <f>'ShareOfInflow-SEIS'!K19</f>
         <v>0.19700563296768453</v>
       </c>
     </row>
@@ -5113,14 +4996,14 @@
         <v>5.981122</v>
       </c>
       <c r="C90" t="str">
-        <f>'ShareOfInflow-SEIS'!$H$10</f>
+        <f>'ShareOfInflow-SEIS'!$H$11</f>
         <v>Alternative 2</v>
       </c>
       <c r="D90" t="s">
         <v>4</v>
       </c>
       <c r="E90" s="56">
-        <f>'ShareOfInflow-SEIS'!K19</f>
+        <f>'ShareOfInflow-SEIS'!K20</f>
         <v>0.18443239987955437</v>
       </c>
     </row>
@@ -5134,14 +5017,14 @@
         <v>10.857008</v>
       </c>
       <c r="C91" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D91" t="s">
         <v>4</v>
       </c>
       <c r="E91" s="56">
-        <f>'ShareOfInflow-SEIS'!P12</f>
+        <f>'ShareOfInflow-SEIS'!P13</f>
         <v>0.17046383923355535</v>
       </c>
     </row>
@@ -5155,14 +5038,14 @@
         <v>9.6009879999900001</v>
       </c>
       <c r="C92" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D92" t="s">
         <v>4</v>
       </c>
       <c r="E92" s="56">
-        <f>'ShareOfInflow-SEIS'!P13</f>
+        <f>'ShareOfInflow-SEIS'!P14</f>
         <v>0.18079959256429842</v>
       </c>
     </row>
@@ -5176,14 +5059,14 @@
         <v>7.6828779999999997</v>
       </c>
       <c r="C93" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D93" t="s">
         <v>4</v>
       </c>
       <c r="E93" s="56">
-        <f>'ShareOfInflow-SEIS'!P14</f>
+        <f>'ShareOfInflow-SEIS'!P15</f>
         <v>0.18219785956669277</v>
       </c>
     </row>
@@ -5197,14 +5080,14 @@
         <v>7.3260519999999998</v>
       </c>
       <c r="C94" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D94" t="s">
         <v>4</v>
       </c>
       <c r="E94" s="56">
-        <f>'ShareOfInflow-SEIS'!P15</f>
+        <f>'ShareOfInflow-SEIS'!P16</f>
         <v>0.19016853932584271</v>
       </c>
     </row>
@@ -5218,14 +5101,14 @@
         <v>6.977665</v>
       </c>
       <c r="C95" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D95" t="s">
         <v>4</v>
       </c>
       <c r="E95" s="56">
-        <f>'ShareOfInflow-SEIS'!P16</f>
+        <f>'ShareOfInflow-SEIS'!P17</f>
         <v>0.19195664575014262</v>
       </c>
     </row>
@@ -5239,14 +5122,14 @@
         <v>6.6375080000000004</v>
       </c>
       <c r="C96" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D96" t="s">
         <v>4</v>
       </c>
       <c r="E96" s="56">
-        <f>'ShareOfInflow-SEIS'!P17</f>
+        <f>'ShareOfInflow-SEIS'!P18</f>
         <v>0.19380069524913096</v>
       </c>
     </row>
@@ -5260,14 +5143,14 @@
         <v>6.305377</v>
       </c>
       <c r="C97" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D97" t="s">
         <v>4</v>
       </c>
       <c r="E97" s="56">
-        <f>'ShareOfInflow-SEIS'!P18</f>
+        <f>'ShareOfInflow-SEIS'!P19</f>
         <v>0.19558498896247239</v>
       </c>
     </row>
@@ -5281,14 +5164,14 @@
         <v>5.981122</v>
       </c>
       <c r="C98" t="str">
-        <f>'ShareOfInflow-SEIS'!$M$10</f>
+        <f>'ShareOfInflow-SEIS'!$M$11</f>
         <v>Interim Guidelines + Drought Contingency Plan</v>
       </c>
       <c r="D98" t="s">
         <v>4</v>
       </c>
       <c r="E98" s="56">
-        <f>'ShareOfInflow-SEIS'!P19</f>
+        <f>'ShareOfInflow-SEIS'!P20</f>
         <v>0.18773946360153257</v>
       </c>
     </row>
@@ -5300,10 +5183,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65016FDA-A485-46B3-A579-17A4BB86DCC0}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5350,710 +5233,730 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="77">
+        <f>C9/$G$9</f>
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="D10" s="77">
+        <f t="shared" ref="D10:G10" si="0">D9/$G$9</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="E10" s="77">
+        <f t="shared" si="0"/>
+        <v>0.48888888888888893</v>
+      </c>
+      <c r="F10" s="77">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G10" s="77">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B11" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="59" t="str">
+      <c r="C11" s="62" t="str">
         <f>'SEIS-Cuts'!I7</f>
         <v>Alternative 1 - Priority</v>
       </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="60" t="s">
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="61" t="s">
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="61"/>
-      <c r="O10" s="61"/>
-      <c r="P10" s="61"/>
-      <c r="Q10" s="61"/>
-    </row>
-    <row r="11" spans="1:17" s="21" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="62"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="51" t="s">
+      <c r="N11" s="64"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="64"/>
+      <c r="Q11" s="64"/>
+    </row>
+    <row r="12" spans="1:17" s="21" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="65"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D12" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="51" t="s">
+      <c r="E12" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="51" t="s">
+      <c r="F12" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="51" t="s">
+      <c r="G12" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="53" t="str">
-        <f>C11</f>
+      <c r="H12" s="53" t="str">
+        <f>C12</f>
         <v>Arizona</v>
       </c>
-      <c r="I11" s="53" t="str">
-        <f t="shared" ref="I11:L11" si="0">D11</f>
+      <c r="I12" s="53" t="str">
+        <f t="shared" ref="I12:L12" si="1">D12</f>
         <v>Nevada</v>
       </c>
-      <c r="J11" s="53" t="str">
-        <f t="shared" si="0"/>
+      <c r="J12" s="53" t="str">
+        <f t="shared" si="1"/>
         <v>California</v>
       </c>
-      <c r="K11" s="53" t="str">
-        <f t="shared" si="0"/>
+      <c r="K12" s="53" t="str">
+        <f t="shared" si="1"/>
         <v>Mexico</v>
       </c>
-      <c r="L11" s="53" t="str">
-        <f t="shared" si="0"/>
+      <c r="L12" s="53" t="str">
+        <f t="shared" si="1"/>
         <v>Total</v>
       </c>
-      <c r="M11" s="45" t="str">
-        <f>H11</f>
+      <c r="M12" s="45" t="str">
+        <f>H12</f>
         <v>Arizona</v>
       </c>
-      <c r="N11" s="45" t="str">
-        <f t="shared" ref="N11" si="1">I11</f>
+      <c r="N12" s="45" t="str">
+        <f t="shared" ref="N12" si="2">I12</f>
         <v>Nevada</v>
       </c>
-      <c r="O11" s="45" t="str">
-        <f t="shared" ref="O11" si="2">J11</f>
+      <c r="O12" s="45" t="str">
+        <f t="shared" ref="O12" si="3">J12</f>
         <v>California</v>
       </c>
-      <c r="P11" s="45" t="str">
-        <f t="shared" ref="P11" si="3">K11</f>
+      <c r="P12" s="45" t="str">
+        <f t="shared" ref="P12" si="4">K12</f>
         <v>Mexico</v>
       </c>
-      <c r="Q11" s="45" t="str">
-        <f t="shared" ref="Q11" si="4">L11</f>
+      <c r="Q12" s="45" t="str">
+        <f t="shared" ref="Q12" si="5">L12</f>
         <v>Total</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" s="49" t="str">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="49" t="str">
         <f>'SEIS-Cuts'!A10</f>
         <v>1,090–&gt;1,075</v>
       </c>
-      <c r="B12" s="50">
+      <c r="B13" s="50">
         <f>'SEIS-Cuts'!B10</f>
         <v>10.857008</v>
       </c>
-      <c r="C12" s="52">
+      <c r="C13" s="52">
         <f>(C$9-'SEIS-Cuts'!O10/1000)/($G$9-'SEIS-Cuts'!$T10/1000)</f>
         <v>0.2822759668185536</v>
       </c>
-      <c r="D12" s="52">
+      <c r="D13" s="52">
         <f>(D$9-'SEIS-Cuts'!P10/1000)/($G$9-'SEIS-Cuts'!$T10/1000)</f>
         <v>3.3181446430657784E-2</v>
       </c>
-      <c r="E12" s="52">
+      <c r="E13" s="52">
         <f>(E$9-'SEIS-Cuts'!Q10/1000)/($G$9-'SEIS-Cuts'!$T10/1000)</f>
         <v>0.51407874751723337</v>
       </c>
-      <c r="F12" s="52">
+      <c r="F13" s="52">
         <f>(F$9-'SEIS-Cuts'!S10/1000)/($G$9-'SEIS-Cuts'!$T10/1000)</f>
         <v>0.17046383923355535</v>
       </c>
-      <c r="G12" s="52">
+      <c r="G13" s="52">
         <f>(G$9-'SEIS-Cuts'!T10)/($G$9-SUM('SEIS-Cuts'!O10:Q10,'SEIS-Cuts'!S10))</f>
         <v>1</v>
       </c>
-      <c r="H12" s="54">
+      <c r="H13" s="54">
         <f>(C$9-'SEIS-Cuts'!Z10/1000)/($G$9-'SEIS-Cuts'!$AE10/1000)</f>
         <v>0.29594578805935273</v>
       </c>
-      <c r="I12" s="54">
+      <c r="I13" s="54">
         <f>(D$9-'SEIS-Cuts'!AA10/1000)/($G$9-'SEIS-Cuts'!$AE10/1000)</f>
         <v>3.3181446430657784E-2</v>
       </c>
-      <c r="J12" s="54">
+      <c r="J13" s="54">
         <f>(E$9-'SEIS-Cuts'!AB10/1000)/($G$9-'SEIS-Cuts'!$AE10/1000)</f>
         <v>0.5004089262764343</v>
       </c>
-      <c r="K12" s="54">
+      <c r="K13" s="54">
         <f>(F$9-'SEIS-Cuts'!AD10/1000)/($G$9-'SEIS-Cuts'!$AE10/1000)</f>
         <v>0.17046383923355535</v>
       </c>
-      <c r="L12" s="54">
+      <c r="L13" s="54">
         <f>(G$9-'SEIS-Cuts'!AE10/1000)/($G$9-'SEIS-Cuts'!$AE10/1000)</f>
         <v>1</v>
       </c>
-      <c r="M12" s="23">
+      <c r="M13" s="23">
         <f>(C$9-'SEIS-Cuts'!C10/1000)/($G$9-'SEIS-Cuts'!$H10/1000)</f>
         <v>0.30470849398294192</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N13" s="23">
         <f>(D$9-'SEIS-Cuts'!D10/1000)/($G$9-'SEIS-Cuts'!$H10/1000)</f>
         <v>3.4116135062507304E-2</v>
       </c>
-      <c r="O12" s="23">
+      <c r="O13" s="23">
         <f>(E$9-'SEIS-Cuts'!E10/1000)/($G$9-'SEIS-Cuts'!$H10/1000)</f>
         <v>0.51407874751723337</v>
       </c>
-      <c r="P12" s="23">
+      <c r="P13" s="23">
         <f>(F$9-'SEIS-Cuts'!G10/1000)/($G$9-'SEIS-Cuts'!$H10/1000)</f>
         <v>0.17046383923355535</v>
       </c>
-      <c r="Q12" s="23">
+      <c r="Q13" s="23">
         <f>(G$9-'SEIS-Cuts'!H10/1000)/($G$9-'SEIS-Cuts'!$H10/1000)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="49" t="str">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="49" t="str">
         <f>'SEIS-Cuts'!A11</f>
         <v>1,075–1,050</v>
       </c>
-      <c r="B13" s="50">
+      <c r="B14" s="50">
         <f>'SEIS-Cuts'!B11</f>
         <v>9.6009879999900001</v>
       </c>
-      <c r="C13" s="52">
+      <c r="C14" s="52">
         <f>(C$9-'SEIS-Cuts'!O11/1000)/($G$9-'SEIS-Cuts'!$T11/1000)</f>
         <v>0.22625413801884389</v>
       </c>
-      <c r="D13" s="52">
+      <c r="D14" s="52">
         <f>(D$9-'SEIS-Cuts'!P11/1000)/($G$9-'SEIS-Cuts'!$T11/1000)</f>
         <v>3.2722179781003308E-2</v>
       </c>
-      <c r="E13" s="52">
+      <c r="E14" s="52">
         <f>(E$9-'SEIS-Cuts'!Q11/1000)/($G$9-'SEIS-Cuts'!$T11/1000)</f>
         <v>0.56022408963585435</v>
       </c>
-      <c r="F13" s="52">
+      <c r="F14" s="52">
         <f>(F$9-'SEIS-Cuts'!S11/1000)/($G$9-'SEIS-Cuts'!$T11/1000)</f>
         <v>0.18079959256429842</v>
       </c>
-      <c r="G13" s="52">
+      <c r="G14" s="52">
         <f>(G$9-'SEIS-Cuts'!T11)/($G$9-SUM('SEIS-Cuts'!O11:Q11,'SEIS-Cuts'!S11))</f>
         <v>1</v>
       </c>
-      <c r="H13" s="54">
+      <c r="H14" s="54">
         <f>(C$9-'SEIS-Cuts'!Z11/1000)/($G$9-'SEIS-Cuts'!$AE11/1000)</f>
         <v>0.26597911892029541</v>
       </c>
-      <c r="I13" s="54">
+      <c r="I14" s="54">
         <f>(D$9-'SEIS-Cuts'!AA11/1000)/($G$9-'SEIS-Cuts'!$AE11/1000)</f>
         <v>3.2849503437738729E-2</v>
       </c>
-      <c r="J13" s="54">
+      <c r="J14" s="54">
         <f>(E$9-'SEIS-Cuts'!AB11/1000)/($G$9-'SEIS-Cuts'!$AE11/1000)</f>
         <v>0.52037178507766746</v>
       </c>
-      <c r="K13" s="54">
+      <c r="K14" s="54">
         <f>(F$9-'SEIS-Cuts'!AD11/1000)/($G$9-'SEIS-Cuts'!$AE11/1000)</f>
         <v>0.18079959256429842</v>
       </c>
-      <c r="L13" s="54">
+      <c r="L14" s="54">
         <f>(G$9-'SEIS-Cuts'!AE11/1000)/($G$9-'SEIS-Cuts'!$AE11/1000)</f>
         <v>1</v>
       </c>
-      <c r="M13" s="23">
+      <c r="M14" s="23">
         <f>(C$9-'SEIS-Cuts'!C11/1000)/($G$9-'SEIS-Cuts'!$H11/1000)</f>
         <v>0.29131652661064422</v>
       </c>
-      <c r="N13" s="23">
+      <c r="N14" s="23">
         <f>(D$9-'SEIS-Cuts'!D11/1000)/($G$9-'SEIS-Cuts'!$H11/1000)</f>
         <v>3.5523300229182576E-2</v>
       </c>
-      <c r="O13" s="23">
+      <c r="O14" s="23">
         <f>(E$9-'SEIS-Cuts'!E11/1000)/($G$9-'SEIS-Cuts'!$H11/1000)</f>
         <v>0.56022408963585435</v>
       </c>
-      <c r="P13" s="23">
+      <c r="P14" s="23">
         <f>(F$9-'SEIS-Cuts'!G11/1000)/($G$9-'SEIS-Cuts'!$H11/1000)</f>
         <v>0.18079959256429842</v>
       </c>
-      <c r="Q13" s="23">
+      <c r="Q14" s="23">
         <f>(G$9-'SEIS-Cuts'!H11/1000)/($G$9-'SEIS-Cuts'!$H11/1000)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A14" s="49" t="str">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="49" t="str">
         <f>'SEIS-Cuts'!A12</f>
         <v>&lt;1,050–&gt;1,045</v>
       </c>
-      <c r="B14" s="50">
+      <c r="B15" s="50">
         <f>'SEIS-Cuts'!B12</f>
         <v>7.6828779999999997</v>
       </c>
-      <c r="C14" s="52">
+      <c r="C15" s="52">
         <f>(C$9-'SEIS-Cuts'!O12/1000)/($G$9-'SEIS-Cuts'!$T12/1000)</f>
         <v>0.2107804750717828</v>
       </c>
-      <c r="D14" s="52">
+      <c r="D15" s="52">
         <f>(D$9-'SEIS-Cuts'!P12/1000)/($G$9-'SEIS-Cuts'!$T12/1000)</f>
         <v>3.2759070738710518E-2</v>
       </c>
-      <c r="E14" s="52">
+      <c r="E15" s="52">
         <f>(E$9-'SEIS-Cuts'!Q12/1000)/($G$9-'SEIS-Cuts'!$T12/1000)</f>
         <v>0.57426259462281393</v>
       </c>
-      <c r="F14" s="52">
+      <c r="F15" s="52">
         <f>(F$9-'SEIS-Cuts'!S12/1000)/($G$9-'SEIS-Cuts'!$T12/1000)</f>
         <v>0.18219785956669277</v>
       </c>
-      <c r="G14" s="52">
+      <c r="G15" s="52">
         <f>(G$9-'SEIS-Cuts'!T12)/($G$9-SUM('SEIS-Cuts'!O12:Q12,'SEIS-Cuts'!S12))</f>
         <v>1</v>
       </c>
-      <c r="H14" s="54">
+      <c r="H15" s="54">
         <f>(C$9-'SEIS-Cuts'!Z12/1000)/($G$9-'SEIS-Cuts'!$AE12/1000)</f>
         <v>0.25815713912816496</v>
       </c>
-      <c r="I14" s="54">
+      <c r="I15" s="54">
         <f>(D$9-'SEIS-Cuts'!AA12/1000)/($G$9-'SEIS-Cuts'!$AE12/1000)</f>
         <v>3.2628556512659883E-2</v>
       </c>
-      <c r="J14" s="54">
+      <c r="J15" s="54">
         <f>(E$9-'SEIS-Cuts'!AB12/1000)/($G$9-'SEIS-Cuts'!$AE12/1000)</f>
         <v>0.52701644479248244</v>
       </c>
-      <c r="K14" s="54">
+      <c r="K15" s="54">
         <f>(F$9-'SEIS-Cuts'!AD12/1000)/($G$9-'SEIS-Cuts'!$AE12/1000)</f>
         <v>0.18219785956669277</v>
       </c>
-      <c r="L14" s="54">
+      <c r="L15" s="54">
         <f>(G$9-'SEIS-Cuts'!AE12/1000)/($G$9-'SEIS-Cuts'!$AE12/1000)</f>
         <v>1</v>
       </c>
-      <c r="M14" s="23">
+      <c r="M15" s="23">
         <f>(C$9-'SEIS-Cuts'!C12/1000)/($G$9-'SEIS-Cuts'!$H12/1000)</f>
         <v>0.28817541111981204</v>
       </c>
-      <c r="N14" s="23">
+      <c r="N15" s="23">
         <f>(D$9-'SEIS-Cuts'!D12/1000)/($G$9-'SEIS-Cuts'!$H12/1000)</f>
         <v>3.5891412163925863E-2</v>
       </c>
-      <c r="O14" s="23">
+      <c r="O15" s="23">
         <f>(E$9-'SEIS-Cuts'!E12/1000)/($G$9-'SEIS-Cuts'!$H12/1000)</f>
         <v>0.57426259462281393</v>
       </c>
-      <c r="P14" s="23">
+      <c r="P15" s="23">
         <f>(F$9-'SEIS-Cuts'!G12/1000)/($G$9-'SEIS-Cuts'!$H12/1000)</f>
         <v>0.18219785956669277</v>
       </c>
-      <c r="Q14" s="23">
+      <c r="Q15" s="23">
         <f>(G$9-'SEIS-Cuts'!H12/1000)/($G$9-'SEIS-Cuts'!$H12/1000)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="49" t="str">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="49" t="str">
         <f>'SEIS-Cuts'!A13</f>
         <v>1,045–&gt;1,040</v>
       </c>
-      <c r="B15" s="50">
+      <c r="B16" s="50">
         <f>'SEIS-Cuts'!B13</f>
         <v>7.3260519999999998</v>
       </c>
-      <c r="C15" s="52">
+      <c r="C16" s="52">
         <f>(C$9-'SEIS-Cuts'!O13/1000)/($G$9-'SEIS-Cuts'!$T13/1000)</f>
         <v>0.16401734104046239</v>
       </c>
-      <c r="D15" s="52">
+      <c r="D16" s="52">
         <f>(D$9-'SEIS-Cuts'!P13/1000)/($G$9-'SEIS-Cuts'!$T13/1000)</f>
         <v>3.3381502890173408E-2</v>
       </c>
-      <c r="E15" s="52">
+      <c r="E16" s="52">
         <f>(E$9-'SEIS-Cuts'!Q13/1000)/($G$9-'SEIS-Cuts'!$T13/1000)</f>
         <v>0.60693641618497118</v>
       </c>
-      <c r="F15" s="52">
+      <c r="F16" s="52">
         <f>(F$9-'SEIS-Cuts'!S13/1000)/($G$9-'SEIS-Cuts'!$T13/1000)</f>
         <v>0.19566473988439309</v>
       </c>
-      <c r="G15" s="52">
+      <c r="G16" s="52">
         <f>(G$9-'SEIS-Cuts'!T13)/($G$9-SUM('SEIS-Cuts'!O13:Q13,'SEIS-Cuts'!S13))</f>
         <v>1</v>
       </c>
-      <c r="H15" s="54">
+      <c r="H16" s="54">
         <f>(C$9-'SEIS-Cuts'!Z13/1000)/($G$9-'SEIS-Cuts'!$AE13/1000)</f>
         <v>0.25786516853932584</v>
       </c>
-      <c r="I15" s="54">
+      <c r="I16" s="54">
         <f>(D$9-'SEIS-Cuts'!AA13/1000)/($G$9-'SEIS-Cuts'!$AE13/1000)</f>
         <v>3.3426966292134833E-2</v>
       </c>
-      <c r="J15" s="54">
+      <c r="J16" s="54">
         <f>(E$9-'SEIS-Cuts'!AB13/1000)/($G$9-'SEIS-Cuts'!$AE13/1000)</f>
         <v>0.51839887640449445</v>
       </c>
-      <c r="K15" s="54">
+      <c r="K16" s="54">
         <f>(F$9-'SEIS-Cuts'!AD13/1000)/($G$9-'SEIS-Cuts'!$AE13/1000)</f>
         <v>0.19016853932584271</v>
       </c>
-      <c r="L15" s="54">
+      <c r="L16" s="54">
         <f>(G$9-'SEIS-Cuts'!AE13/1000)/($G$9-'SEIS-Cuts'!$AE13/1000)</f>
         <v>1</v>
       </c>
-      <c r="M15" s="23">
+      <c r="M16" s="23">
         <f>(C$9-'SEIS-Cuts'!C13/1000)/($G$9-'SEIS-Cuts'!$H13/1000)</f>
         <v>0.3033707865168539</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N16" s="23">
         <f>(D$9-'SEIS-Cuts'!D13/1000)/($G$9-'SEIS-Cuts'!$H13/1000)</f>
         <v>3.8342696629213475E-2</v>
       </c>
-      <c r="O15" s="23">
+      <c r="O16" s="23">
         <f>(E$9-'SEIS-Cuts'!E13/1000)/($G$9-'SEIS-Cuts'!$H13/1000)</f>
         <v>0.5898876404494382</v>
       </c>
-      <c r="P15" s="23">
+      <c r="P16" s="23">
         <f>(F$9-'SEIS-Cuts'!G13/1000)/($G$9-'SEIS-Cuts'!$H13/1000)</f>
         <v>0.19016853932584271</v>
       </c>
-      <c r="Q15" s="23">
+      <c r="Q16" s="23">
         <f>(G$9-'SEIS-Cuts'!H13/1000)/($G$9-'SEIS-Cuts'!$H13/1000)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A16" s="49" t="str">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" s="49" t="str">
         <f>'SEIS-Cuts'!A14</f>
         <v>1,040–&gt;1,035</v>
       </c>
-      <c r="B16" s="50">
+      <c r="B17" s="50">
         <f>'SEIS-Cuts'!B14</f>
         <v>6.977665</v>
       </c>
-      <c r="C16" s="52">
+      <c r="C17" s="52">
         <f>(C$9-'SEIS-Cuts'!O14/1000)/($G$9-'SEIS-Cuts'!$T14/1000)</f>
         <v>0.15703090344521659</v>
       </c>
-      <c r="D16" s="52">
+      <c r="D17" s="52">
         <f>(D$9-'SEIS-Cuts'!P14/1000)/($G$9-'SEIS-Cuts'!$T14/1000)</f>
         <v>3.2086352210557438E-2</v>
       </c>
-      <c r="E16" s="52">
+      <c r="E17" s="52">
         <f>(E$9-'SEIS-Cuts'!Q14/1000)/($G$9-'SEIS-Cuts'!$T14/1000)</f>
         <v>0.6118586426142244</v>
       </c>
-      <c r="F16" s="52">
+      <c r="F17" s="52">
         <f>(F$9-'SEIS-Cuts'!S14/1000)/($G$9-'SEIS-Cuts'!$T14/1000)</f>
         <v>0.19902410173000148</v>
       </c>
-      <c r="G16" s="52">
+      <c r="G17" s="52">
         <f>(G$9-'SEIS-Cuts'!T14)/($G$9-SUM('SEIS-Cuts'!O14:Q14,'SEIS-Cuts'!S14))</f>
         <v>1</v>
       </c>
-      <c r="H16" s="54">
+      <c r="H17" s="54">
         <f>(C$9-'SEIS-Cuts'!Z14/1000)/($G$9-'SEIS-Cuts'!$AE14/1000)</f>
         <v>0.25506432056779532</v>
       </c>
-      <c r="I16" s="54">
+      <c r="I17" s="54">
         <f>(D$9-'SEIS-Cuts'!AA14/1000)/($G$9-'SEIS-Cuts'!$AE14/1000)</f>
         <v>3.3417122578737246E-2</v>
       </c>
-      <c r="J16" s="54">
+      <c r="J17" s="54">
         <f>(E$9-'SEIS-Cuts'!AB14/1000)/($G$9-'SEIS-Cuts'!$AE14/1000)</f>
         <v>0.51249445512346592</v>
       </c>
-      <c r="K16" s="54">
+      <c r="K17" s="54">
         <f>(F$9-'SEIS-Cuts'!AD14/1000)/($G$9-'SEIS-Cuts'!$AE14/1000)</f>
         <v>0.19902410173000148</v>
       </c>
-      <c r="L16" s="54">
+      <c r="L17" s="54">
         <f>(G$9-'SEIS-Cuts'!AE14/1000)/($G$9-'SEIS-Cuts'!$AE14/1000)</f>
         <v>1</v>
       </c>
-      <c r="M16" s="23">
+      <c r="M17" s="23">
         <f>(C$9-'SEIS-Cuts'!C14/1000)/($G$9-'SEIS-Cuts'!$H14/1000)</f>
         <v>0.30804335424985735</v>
       </c>
-      <c r="N16" s="23">
+      <c r="N17" s="23">
         <f>(D$9-'SEIS-Cuts'!D14/1000)/($G$9-'SEIS-Cuts'!$H14/1000)</f>
         <v>3.8933257273245855E-2</v>
       </c>
-      <c r="O16" s="23">
+      <c r="O17" s="23">
         <f>(E$9-'SEIS-Cuts'!E14/1000)/($G$9-'SEIS-Cuts'!$H14/1000)</f>
         <v>0.59184255561893895</v>
       </c>
-      <c r="P16" s="23">
+      <c r="P17" s="23">
         <f>(F$9-'SEIS-Cuts'!G14/1000)/($G$9-'SEIS-Cuts'!$H14/1000)</f>
         <v>0.19195664575014262</v>
       </c>
-      <c r="Q16" s="23">
+      <c r="Q17" s="23">
         <f>(G$9-'SEIS-Cuts'!H14/1000)/($G$9-'SEIS-Cuts'!$H14/1000)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A17" s="49" t="str">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" s="49" t="str">
         <f>'SEIS-Cuts'!A15</f>
         <v>1,035–&gt;1,030</v>
       </c>
-      <c r="B17" s="50">
+      <c r="B18" s="50">
         <f>'SEIS-Cuts'!B15</f>
         <v>6.6375080000000004</v>
       </c>
-      <c r="C17" s="52">
+      <c r="C18" s="52">
         <f>(C$9-'SEIS-Cuts'!O15/1000)/($G$9-'SEIS-Cuts'!$T15/1000)</f>
         <v>0.15810629745422058</v>
       </c>
-      <c r="D17" s="52">
+      <c r="D18" s="52">
         <f>(D$9-'SEIS-Cuts'!P15/1000)/($G$9-'SEIS-Cuts'!$T15/1000)</f>
         <v>3.2306089027839803E-2</v>
       </c>
-      <c r="E17" s="52">
+      <c r="E18" s="52">
         <f>(E$9-'SEIS-Cuts'!Q15/1000)/($G$9-'SEIS-Cuts'!$T15/1000)</f>
         <v>0.61039154384397798</v>
       </c>
-      <c r="F17" s="52">
+      <c r="F18" s="52">
         <f>(F$9-'SEIS-Cuts'!S15/1000)/($G$9-'SEIS-Cuts'!$T15/1000)</f>
         <v>0.19919606967396158</v>
       </c>
-      <c r="G17" s="52">
+      <c r="G18" s="52">
         <f>(G$9-'SEIS-Cuts'!T15)/($G$9-SUM('SEIS-Cuts'!O15:Q15,'SEIS-Cuts'!S15))</f>
         <v>1</v>
       </c>
-      <c r="H17" s="54">
+      <c r="H18" s="54">
         <f>(C$9-'SEIS-Cuts'!Z15/1000)/($G$9-'SEIS-Cuts'!$AE15/1000)</f>
         <v>0.25803108808290154</v>
       </c>
-      <c r="I17" s="54">
+      <c r="I18" s="54">
         <f>(D$9-'SEIS-Cuts'!AA15/1000)/($G$9-'SEIS-Cuts'!$AE15/1000)</f>
         <v>3.3752775721687639E-2</v>
       </c>
-      <c r="J17" s="54">
+      <c r="J18" s="54">
         <f>(E$9-'SEIS-Cuts'!AB15/1000)/($G$9-'SEIS-Cuts'!$AE15/1000)</f>
         <v>0.50999259807549968</v>
       </c>
-      <c r="K17" s="54">
+      <c r="K18" s="54">
         <f>(F$9-'SEIS-Cuts'!AD15/1000)/($G$9-'SEIS-Cuts'!$AE15/1000)</f>
         <v>0.19807549962990378</v>
       </c>
-      <c r="L17" s="54">
+      <c r="L18" s="54">
         <f>(G$9-'SEIS-Cuts'!AE15/1000)/($G$9-'SEIS-Cuts'!$AE15/1000)</f>
         <v>1</v>
       </c>
-      <c r="M17" s="23">
+      <c r="M18" s="23">
         <f>(C$9-'SEIS-Cuts'!C15/1000)/($G$9-'SEIS-Cuts'!$H15/1000)</f>
         <v>0.31286210892236382</v>
       </c>
-      <c r="N17" s="23">
+      <c r="N18" s="23">
         <f>(D$9-'SEIS-Cuts'!D15/1000)/($G$9-'SEIS-Cuts'!$H15/1000)</f>
         <v>3.9542294322132091E-2</v>
       </c>
-      <c r="O17" s="23">
+      <c r="O18" s="23">
         <f>(E$9-'SEIS-Cuts'!E15/1000)/($G$9-'SEIS-Cuts'!$H15/1000)</f>
         <v>0.59385863267670924</v>
       </c>
-      <c r="P17" s="23">
+      <c r="P18" s="23">
         <f>(F$9-'SEIS-Cuts'!G15/1000)/($G$9-'SEIS-Cuts'!$H15/1000)</f>
         <v>0.19380069524913096</v>
       </c>
-      <c r="Q17" s="23">
+      <c r="Q18" s="23">
         <f>(G$9-'SEIS-Cuts'!H15/1000)/($G$9-'SEIS-Cuts'!$H15/1000)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A18" s="49" t="str">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" s="49" t="str">
         <f>'SEIS-Cuts'!A16</f>
         <v>1,030–1,025</v>
       </c>
-      <c r="B18" s="50">
+      <c r="B19" s="50">
         <f>'SEIS-Cuts'!B16</f>
         <v>6.305377</v>
       </c>
-      <c r="C18" s="52">
+      <c r="C19" s="52">
         <f>(C$9-'SEIS-Cuts'!O16/1000)/($G$9-'SEIS-Cuts'!$T16/1000)</f>
         <v>0.15950735956743767</v>
       </c>
-      <c r="D18" s="52">
+      <c r="D19" s="52">
         <f>(D$9-'SEIS-Cuts'!P16/1000)/($G$9-'SEIS-Cuts'!$T16/1000)</f>
         <v>3.2592370081105437E-2</v>
       </c>
-      <c r="E18" s="52">
+      <c r="E19" s="52">
         <f>(E$9-'SEIS-Cuts'!Q16/1000)/($G$9-'SEIS-Cuts'!$T16/1000)</f>
         <v>0.60829077801141496</v>
       </c>
-      <c r="F18" s="52">
+      <c r="F19" s="52">
         <f>(F$9-'SEIS-Cuts'!S16/1000)/($G$9-'SEIS-Cuts'!$T16/1000)</f>
         <v>0.19960949234004208</v>
       </c>
-      <c r="G18" s="52">
+      <c r="G19" s="52">
         <f>(G$9-'SEIS-Cuts'!T16)/($G$9-SUM('SEIS-Cuts'!O16:Q16,'SEIS-Cuts'!S16))</f>
         <v>1</v>
       </c>
-      <c r="H18" s="54">
+      <c r="H19" s="54">
         <f>(C$9-'SEIS-Cuts'!Z16/1000)/($G$9-'SEIS-Cuts'!$AE16/1000)</f>
         <v>0.26119181737325819</v>
       </c>
-      <c r="I18" s="54">
+      <c r="I19" s="54">
         <f>(D$9-'SEIS-Cuts'!AA16/1000)/($G$9-'SEIS-Cuts'!$AE16/1000)</f>
         <v>3.4094278090720423E-2</v>
       </c>
-      <c r="J18" s="54">
+      <c r="J19" s="54">
         <f>(E$9-'SEIS-Cuts'!AB16/1000)/($G$9-'SEIS-Cuts'!$AE16/1000)</f>
         <v>0.50770827156833676</v>
       </c>
-      <c r="K18" s="54">
+      <c r="K19" s="54">
         <f>(F$9-'SEIS-Cuts'!AD16/1000)/($G$9-'SEIS-Cuts'!$AE16/1000)</f>
         <v>0.19700563296768453</v>
       </c>
-      <c r="L18" s="54">
+      <c r="L19" s="54">
         <f>(G$9-'SEIS-Cuts'!AE16/1000)/($G$9-'SEIS-Cuts'!$AE16/1000)</f>
         <v>1</v>
       </c>
-      <c r="M18" s="23">
+      <c r="M19" s="23">
         <f>(C$9-'SEIS-Cuts'!C16/1000)/($G$9-'SEIS-Cuts'!$H16/1000)</f>
         <v>0.31788079470198671</v>
       </c>
-      <c r="N18" s="23">
+      <c r="N19" s="23">
         <f>(D$9-'SEIS-Cuts'!D16/1000)/($G$9-'SEIS-Cuts'!$H16/1000)</f>
         <v>4.0176600441501099E-2</v>
       </c>
-      <c r="O18" s="23">
+      <c r="O19" s="23">
         <f>(E$9-'SEIS-Cuts'!E16/1000)/($G$9-'SEIS-Cuts'!$H16/1000)</f>
         <v>0.59602649006622532</v>
       </c>
-      <c r="P18" s="23">
+      <c r="P19" s="23">
         <f>(F$9-'SEIS-Cuts'!G16/1000)/($G$9-'SEIS-Cuts'!$H16/1000)</f>
         <v>0.19558498896247239</v>
       </c>
-      <c r="Q18" s="23">
+      <c r="Q19" s="23">
         <f>(G$9-'SEIS-Cuts'!H16/1000)/($G$9-'SEIS-Cuts'!$H16/1000)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A19" s="49" t="str">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A20" s="49" t="str">
         <f>'SEIS-Cuts'!A17</f>
         <v>&lt;1,025–1,000</v>
       </c>
-      <c r="B19" s="50">
+      <c r="B20" s="50">
         <f>'SEIS-Cuts'!B17</f>
         <v>5.981122</v>
       </c>
-      <c r="C19" s="52">
+      <c r="C20" s="52">
         <f>(C$9-'SEIS-Cuts'!O17/1000)/($G$9-'SEIS-Cuts'!$T17/1000)</f>
         <v>0.1620384498016478</v>
       </c>
-      <c r="D19" s="52">
+      <c r="D20" s="52">
         <f>(D$9-'SEIS-Cuts'!P17/1000)/($G$9-'SEIS-Cuts'!$T17/1000)</f>
         <v>3.3109551418980768E-2</v>
       </c>
-      <c r="E19" s="52">
+      <c r="E20" s="52">
         <f>(E$9-'SEIS-Cuts'!Q17/1000)/($G$9-'SEIS-Cuts'!$T17/1000)</f>
         <v>0.61794324076899609</v>
       </c>
-      <c r="F19" s="52">
+      <c r="F20" s="52">
         <f>(F$9-'SEIS-Cuts'!S17/1000)/($G$9-'SEIS-Cuts'!$T17/1000)</f>
         <v>0.18690875801037535</v>
       </c>
-      <c r="G19" s="52">
+      <c r="G20" s="52">
         <f>(G$9-'SEIS-Cuts'!T17)/($G$9-SUM('SEIS-Cuts'!O17:Q17,'SEIS-Cuts'!S17))</f>
         <v>1</v>
       </c>
-      <c r="H19" s="54">
+      <c r="H20" s="54">
         <f>(C$9-'SEIS-Cuts'!Z17/1000)/($G$9-'SEIS-Cuts'!$AE17/1000)</f>
         <v>0.25790424570912374</v>
       </c>
-      <c r="I19" s="54">
+      <c r="I20" s="54">
         <f>(D$9-'SEIS-Cuts'!AA17/1000)/($G$9-'SEIS-Cuts'!$AE17/1000)</f>
         <v>3.4778681120144532E-2</v>
       </c>
-      <c r="J19" s="54">
+      <c r="J20" s="54">
         <f>(E$9-'SEIS-Cuts'!AB17/1000)/($G$9-'SEIS-Cuts'!$AE17/1000)</f>
         <v>0.52288467329117749</v>
       </c>
-      <c r="K19" s="54">
+      <c r="K20" s="54">
         <f>(F$9-'SEIS-Cuts'!AD17/1000)/($G$9-'SEIS-Cuts'!$AE17/1000)</f>
         <v>0.18443239987955437</v>
       </c>
-      <c r="L19" s="54">
+      <c r="L20" s="54">
         <f>(G$9-'SEIS-Cuts'!AE17/1000)/($G$9-'SEIS-Cuts'!$AE17/1000)</f>
         <v>1</v>
       </c>
-      <c r="M19" s="23">
+      <c r="M20" s="23">
         <f>(C$9-'SEIS-Cuts'!C17/1000)/($G$9-'SEIS-Cuts'!$H17/1000)</f>
         <v>0.31877394636015327</v>
       </c>
-      <c r="N19" s="23">
+      <c r="N20" s="23">
         <f>(D$9-'SEIS-Cuts'!D17/1000)/($G$9-'SEIS-Cuts'!$H17/1000)</f>
         <v>4.1379310344827586E-2</v>
       </c>
-      <c r="O19" s="23">
+      <c r="O20" s="23">
         <f>(E$9-'SEIS-Cuts'!E17/1000)/($G$9-'SEIS-Cuts'!$H17/1000)</f>
         <v>0.62068965517241392</v>
       </c>
-      <c r="P19" s="23">
+      <c r="P20" s="23">
         <f>(F$9-'SEIS-Cuts'!G17/1000)/($G$9-'SEIS-Cuts'!$H17/1000)</f>
         <v>0.18773946360153257</v>
       </c>
-      <c r="Q19" s="23">
+      <c r="Q20" s="23">
         <f>(G$9-'SEIS-Cuts'!H17/1000)/($G$9-'SEIS-Cuts'!$H17/1000)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A20" s="22" t="str">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="str">
         <f>'SEIS-Cuts'!A18</f>
         <v>&lt;1,000–975</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B21" s="6">
         <f>'SEIS-Cuts'!B18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A21" s="22" t="str">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" s="22" t="str">
         <f>'SEIS-Cuts'!A19</f>
         <v>&lt;975–950</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B22" s="6">
         <f>'SEIS-Cuts'!B19</f>
         <v>0</v>
       </c>
-      <c r="G21" s="46"/>
-      <c r="L21" s="46"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A22" s="22" t="str">
+      <c r="G22" s="46"/>
+      <c r="L22" s="46"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A23" s="22" t="str">
         <f>'SEIS-Cuts'!A20</f>
         <v>&lt;950</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B23" s="6">
         <f>'SEIS-Cuts'!B20</f>
         <v>0</v>
       </c>
-      <c r="G22" s="46"/>
-      <c r="L22" s="46"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="G23" s="46"/>
       <c r="L23" s="46"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
       <c r="G24" s="46"/>
       <c r="L24" s="46"/>
     </row>
-    <row r="25" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
       <c r="G25" s="46"/>
-      <c r="H25" s="48"/>
       <c r="L25" s="46"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
       <c r="G26" s="46"/>
+      <c r="H26" s="48"/>
       <c r="L26" s="46"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.35">
@@ -6066,14 +5969,18 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="G29" s="46"/>
+      <c r="L29" s="46"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="G30" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="M10:Q10"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="M11:Q11"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6148,7 +6055,7 @@
       <c r="A7" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="70" t="s">
         <v>86</v>
       </c>
       <c r="C7" s="67" t="s">
@@ -6159,82 +6066,82 @@
       <c r="F7" s="67"/>
       <c r="G7" s="67"/>
       <c r="H7" s="67"/>
-      <c r="I7" s="66" t="s">
+      <c r="I7" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
-      <c r="O7" s="66"/>
-      <c r="P7" s="66"/>
-      <c r="Q7" s="66"/>
-      <c r="R7" s="66"/>
-      <c r="S7" s="66"/>
-      <c r="T7" s="66"/>
-      <c r="U7" s="66" t="s">
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="V7" s="66"/>
-      <c r="W7" s="66"/>
-      <c r="X7" s="66"/>
-      <c r="Y7" s="66"/>
-      <c r="Z7" s="66"/>
-      <c r="AA7" s="66"/>
-      <c r="AB7" s="66"/>
-      <c r="AC7" s="66"/>
+      <c r="V7" s="74"/>
+      <c r="W7" s="74"/>
+      <c r="X7" s="74"/>
+      <c r="Y7" s="74"/>
+      <c r="Z7" s="74"/>
+      <c r="AA7" s="74"/>
+      <c r="AB7" s="74"/>
+      <c r="AC7" s="74"/>
       <c r="AD7" s="42"/>
       <c r="AE7" s="42"/>
-      <c r="AF7" s="66" t="s">
+      <c r="AF7" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="AG7" s="66"/>
+      <c r="AG7" s="74"/>
     </row>
     <row r="8" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="67"/>
-      <c r="B8" s="72"/>
+      <c r="B8" s="71"/>
       <c r="C8" s="67"/>
       <c r="D8" s="67"/>
       <c r="E8" s="67"/>
       <c r="F8" s="67"/>
       <c r="G8" s="67"/>
       <c r="H8" s="67"/>
-      <c r="I8" s="69" t="s">
+      <c r="I8" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="69" t="s">
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="69"/>
-      <c r="S8" s="69"/>
-      <c r="T8" s="69"/>
-      <c r="U8" s="70" t="s">
+      <c r="P8" s="68"/>
+      <c r="Q8" s="68"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="68"/>
+      <c r="T8" s="68"/>
+      <c r="U8" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="V8" s="70"/>
-      <c r="W8" s="70"/>
-      <c r="X8" s="70"/>
-      <c r="Y8" s="70"/>
-      <c r="Z8" s="64" t="s">
+      <c r="V8" s="69"/>
+      <c r="W8" s="69"/>
+      <c r="X8" s="69"/>
+      <c r="Y8" s="69"/>
+      <c r="Z8" s="72" t="s">
         <v>77</v>
       </c>
-      <c r="AA8" s="68"/>
-      <c r="AB8" s="68"/>
-      <c r="AC8" s="68"/>
-      <c r="AD8" s="68"/>
-      <c r="AE8" s="65"/>
-      <c r="AF8" s="64" t="s">
+      <c r="AA8" s="75"/>
+      <c r="AB8" s="75"/>
+      <c r="AC8" s="75"/>
+      <c r="AD8" s="75"/>
+      <c r="AE8" s="73"/>
+      <c r="AF8" s="72" t="s">
         <v>85</v>
       </c>
-      <c r="AG8" s="65"/>
+      <c r="AG8" s="73"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" s="41"/>
@@ -7778,17 +7685,17 @@
     <sortCondition descending="1" ref="B10:B17"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="I8:N8"/>
-    <mergeCell ref="O8:T8"/>
-    <mergeCell ref="U8:Y8"/>
-    <mergeCell ref="B7:B8"/>
     <mergeCell ref="AF8:AG8"/>
     <mergeCell ref="AF7:AG7"/>
     <mergeCell ref="I7:T7"/>
     <mergeCell ref="U7:AC7"/>
     <mergeCell ref="C7:H8"/>
     <mergeCell ref="Z8:AE8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="O8:T8"/>
+    <mergeCell ref="U8:Y8"/>
+    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{37A0A559-A066-48B0-9816-F9F7E3B09C10}"/>
@@ -7832,25 +7739,25 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="73" t="s">
+      <c r="D3" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73" t="s">
+      <c r="E3" s="76"/>
+      <c r="F3" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73" t="s">
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="M3" s="73" t="s">
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="M3" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
     </row>
     <row r="4" spans="1:16" s="4" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">

</xml_diff>